<commit_message>
Initial keymap and key overrides
Not sure if these key overrides will work, considering some of them are to do with the shift key and shifted keycodes.
</commit_message>
<xml_diff>
--- a/firmware/key_physical_positions.xlsx
+++ b/firmware/key_physical_positions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>SW</t>
   </si>
@@ -27,10 +27,16 @@
     <t xml:space="preserve">y dist from topmost</t>
   </si>
   <si>
-    <t xml:space="preserve">x formula</t>
+    <t xml:space="preserve">rgb x</t>
   </si>
   <si>
-    <t xml:space="preserve">y formula</t>
+    <t xml:space="preserve">rgb y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">key x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">key y</t>
   </si>
   <si>
     <t>MAX_X</t>
@@ -46,6 +52,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <sz val="11.000000"/>
@@ -81,11 +90,16 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="2" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <protection hidden="0" locked="1"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="1" applyFill="1"/>
   </cellXfs>
@@ -609,6 +623,7 @@
     <col bestFit="1" min="3" max="3" width="17.7109375"/>
     <col bestFit="1" min="4" max="4" width="8.7109375"/>
     <col bestFit="1" min="5" max="5" width="8.8515625"/>
+    <col min="6" max="6" width="8.8515625"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
@@ -627,14 +642,20 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2" ht="14.25">
@@ -648,20 +669,28 @@
         <v>30.899999999999999</v>
       </c>
       <c r="D2">
-        <f>ROUND(B2/$G$2*224,1)-1</f>
-        <v>-1</v>
-      </c>
-      <c r="E2" s="1">
-        <f>ROUND(C2/$H$2*64,1)-1</f>
+        <f>MAX(0,ROUND(B2/$H$2*224,1)-1)</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
+        <f>MAX(0,ROUND(C2/$I$2*64,1)-1)</f>
         <v>20</v>
       </c>
-      <c r="G2">
+      <c r="F2" s="3">
+        <f>B2/19</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="4">
+        <f>C2/19</f>
+        <v>1.6263157894736842</v>
+      </c>
+      <c r="H2">
         <v>139.19999999999999</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>94.200000000000003</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>100</v>
       </c>
     </row>
@@ -676,16 +705,24 @@
         <v>29.699999999999999</v>
       </c>
       <c r="D3">
-        <f>ROUND(B3/$G$2*224,1)-1</f>
+        <f>MAX(0,ROUND(B3/$H$2*224,1)-1)</f>
         <v>33.399999999999999</v>
       </c>
-      <c r="E3" s="1">
-        <f>ROUND(C3/$H$2*64,1)-1</f>
+      <c r="E3" s="2">
+        <f>MAX(0,ROUND(C3/$I$2*64,1)-1)</f>
         <v>19.200000000000003</v>
       </c>
+      <c r="F3" s="3">
+        <f>B3/19</f>
+        <v>1.1263157894736842</v>
+      </c>
+      <c r="G3" s="4">
+        <f>C3/19</f>
+        <v>1.5631578947368421</v>
+      </c>
     </row>
     <row r="4" ht="14.25">
-      <c r="A4" s="2">
+      <c r="A4" s="5">
         <v>2</v>
       </c>
       <c r="B4">
@@ -695,16 +732,24 @@
         <v>9.5999999999999996</v>
       </c>
       <c r="D4">
-        <f>ROUND(B4/$G$2*224,1)-1</f>
+        <f>MAX(0,ROUND(B4/$H$2*224,1)-1)</f>
         <v>67.700000000000003</v>
       </c>
-      <c r="E4" s="1">
-        <f>ROUND(C4/$H$2*64,1)-1</f>
+      <c r="E4" s="2">
+        <f>MAX(0,ROUND(C4/$I$2*64,1)-1)</f>
         <v>5.5</v>
       </c>
+      <c r="F4" s="3">
+        <f>B4/19</f>
+        <v>2.2473684210526317</v>
+      </c>
+      <c r="G4" s="4">
+        <f>C4/19</f>
+        <v>0.50526315789473686</v>
+      </c>
     </row>
     <row r="5" ht="14.25">
-      <c r="A5" s="2">
+      <c r="A5" s="5">
         <v>3</v>
       </c>
       <c r="B5">
@@ -714,16 +759,24 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <f>ROUND(B5/$G$2*224,1)-1</f>
+        <f>MAX(0,ROUND(B5/$H$2*224,1)-1)</f>
         <v>100.7</v>
       </c>
-      <c r="E5" s="1">
-        <f>ROUND(C5/$H$2*64,1)-1</f>
-        <v>-1</v>
+      <c r="E5" s="2">
+        <f>MAX(0,ROUND(C5/$I$2*64,1)-1)</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="3">
+        <f>B5/19</f>
+        <v>3.3263157894736843</v>
+      </c>
+      <c r="G5" s="4">
+        <f>C5/19</f>
+        <v>0</v>
       </c>
     </row>
     <row r="6" ht="14.25">
-      <c r="A6" s="2">
+      <c r="A6" s="5">
         <v>4</v>
       </c>
       <c r="B6">
@@ -733,16 +786,24 @@
         <v>16.100000000000001</v>
       </c>
       <c r="D6">
-        <f>ROUND(B6/$G$2*224,1)-1</f>
+        <f>MAX(0,ROUND(B6/$H$2*224,1)-1)</f>
         <v>132.09999999999999</v>
       </c>
-      <c r="E6" s="1">
-        <f>ROUND(C6/$H$2*64,1)-1</f>
+      <c r="E6" s="2">
+        <f>MAX(0,ROUND(C6/$I$2*64,1)-1)</f>
         <v>9.9000000000000004</v>
       </c>
+      <c r="F6" s="3">
+        <f>B6/19</f>
+        <v>4.3526315789473689</v>
+      </c>
+      <c r="G6" s="4">
+        <f>C6/19</f>
+        <v>0.84736842105263166</v>
+      </c>
     </row>
     <row r="7" ht="14.25">
-      <c r="A7" s="2">
+      <c r="A7" s="5">
         <v>5</v>
       </c>
       <c r="B7">
@@ -752,136 +813,192 @@
         <v>18</v>
       </c>
       <c r="D7">
-        <f>ROUND(B7/$G$2*224,1)-1</f>
+        <f>MAX(0,ROUND(B7/$H$2*224,1)-1)</f>
         <v>166.5</v>
       </c>
-      <c r="E7" s="1">
-        <f>ROUND(C7/$H$2*64,1)-1</f>
+      <c r="E7" s="2">
+        <f>MAX(0,ROUND(C7/$I$2*64,1)-1)</f>
         <v>11.200000000000001</v>
       </c>
+      <c r="F7" s="3">
+        <f>B7/19</f>
+        <v>5.4789473684210526</v>
+      </c>
+      <c r="G7" s="4">
+        <f>C7/19</f>
+        <v>0.94736842105263153</v>
+      </c>
     </row>
     <row r="8" ht="14.25">
-      <c r="A8" s="3">
+      <c r="A8" s="6">
         <v>6</v>
       </c>
-      <c r="B8" s="3">
-        <f>$G$2+$I$2+($G$2-B7)</f>
+      <c r="B8" s="6">
+        <f>$H$2+$J$2+($H$2-B7)</f>
         <v>274.29999999999995</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="6">
         <v>18</v>
       </c>
-      <c r="D8" s="3">
-        <f>ROUND(B8/$G$2*224,1)-1</f>
+      <c r="D8">
+        <f>MAX(0,ROUND(B8/$H$2*224,1)-1)</f>
         <v>440.40000000000003</v>
       </c>
-      <c r="E8" s="1">
-        <f>ROUND(C8/$H$2*64,1)-1</f>
+      <c r="E8" s="2">
+        <f>MAX(0,ROUND(C8/$I$2*64,1)-1)</f>
         <v>11.200000000000001</v>
       </c>
+      <c r="F8" s="3">
+        <f>B8/19</f>
+        <v>14.436842105263155</v>
+      </c>
+      <c r="G8" s="4">
+        <f>C8/19</f>
+        <v>0.94736842105263153</v>
+      </c>
     </row>
     <row r="9" ht="14.25">
-      <c r="A9" s="3">
+      <c r="A9" s="6">
         <v>7</v>
       </c>
-      <c r="B9" s="3">
-        <f>$G$2+$I$2+($G$2-B6)</f>
+      <c r="B9" s="6">
+        <f>$H$2+$J$2+($H$2-B6)</f>
         <v>295.69999999999999</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="6">
         <v>16.100000000000001</v>
       </c>
-      <c r="D9" s="3">
-        <f>ROUND(B9/$G$2*224,1)-1</f>
+      <c r="D9">
+        <f>MAX(0,ROUND(B9/$H$2*224,1)-1)</f>
         <v>474.80000000000001</v>
       </c>
-      <c r="E9" s="1">
-        <f>ROUND(C9/$H$2*64,1)-1</f>
+      <c r="E9" s="2">
+        <f>MAX(0,ROUND(C9/$I$2*64,1)-1)</f>
         <v>9.9000000000000004</v>
       </c>
+      <c r="F9" s="3">
+        <f>B9/19</f>
+        <v>15.563157894736841</v>
+      </c>
+      <c r="G9" s="4">
+        <f>C9/19</f>
+        <v>0.84736842105263166</v>
+      </c>
     </row>
     <row r="10" ht="14.25">
-      <c r="A10" s="3">
+      <c r="A10" s="6">
         <v>8</v>
       </c>
-      <c r="B10" s="3">
-        <f>$G$2+$I$2+($G$2-B5)</f>
+      <c r="B10" s="6">
+        <f>$H$2+$J$2+($H$2-B5)</f>
         <v>315.19999999999999</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="6">
         <v>0</v>
       </c>
-      <c r="D10" s="3">
-        <f>ROUND(B10/$G$2*224,1)-1</f>
+      <c r="D10">
+        <f>MAX(0,ROUND(B10/$H$2*224,1)-1)</f>
         <v>506.20000000000005</v>
       </c>
-      <c r="E10" s="1">
-        <f>ROUND(C10/$H$2*64,1)-1</f>
-        <v>-1</v>
+      <c r="E10" s="2">
+        <f>MAX(0,ROUND(C10/$I$2*64,1)-1)</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="3">
+        <f>B10/19</f>
+        <v>16.589473684210525</v>
+      </c>
+      <c r="G10" s="4">
+        <f>C10/19</f>
+        <v>0</v>
       </c>
     </row>
     <row r="11" ht="14.25">
-      <c r="A11" s="3">
+      <c r="A11" s="6">
         <v>9</v>
       </c>
-      <c r="B11" s="3">
-        <f>$G$2+$I$2+($G$2-B4)</f>
+      <c r="B11" s="6">
+        <f>$H$2+$J$2+($H$2-B4)</f>
         <v>335.69999999999999</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="6">
         <v>9.5999999999999996</v>
       </c>
-      <c r="D11" s="3">
-        <f>ROUND(B11/$G$2*224,1)-1</f>
+      <c r="D11">
+        <f>MAX(0,ROUND(B11/$H$2*224,1)-1)</f>
         <v>539.20000000000005</v>
       </c>
-      <c r="E11" s="1">
-        <f>ROUND(C11/$H$2*64,1)-1</f>
+      <c r="E11" s="2">
+        <f>MAX(0,ROUND(C11/$I$2*64,1)-1)</f>
         <v>5.5</v>
       </c>
+      <c r="F11" s="3">
+        <f>B11/19</f>
+        <v>17.668421052631579</v>
+      </c>
+      <c r="G11" s="4">
+        <f>C11/19</f>
+        <v>0.50526315789473686</v>
+      </c>
     </row>
     <row r="12" ht="14.25">
-      <c r="A12" s="3">
+      <c r="A12" s="6">
         <v>10</v>
       </c>
-      <c r="B12" s="3">
-        <f>$G$2+$I$2+($G$2-B3)</f>
+      <c r="B12" s="6">
+        <f>$H$2+$J$2+($H$2-B3)</f>
         <v>357</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="6">
         <v>29.699999999999999</v>
       </c>
-      <c r="D12" s="3">
-        <f>ROUND(B12/$G$2*224,1)-1</f>
+      <c r="D12">
+        <f>MAX(0,ROUND(B12/$H$2*224,1)-1)</f>
         <v>573.5</v>
       </c>
-      <c r="E12" s="1">
-        <f>ROUND(C12/$H$2*64,1)-1</f>
+      <c r="E12" s="2">
+        <f>MAX(0,ROUND(C12/$I$2*64,1)-1)</f>
         <v>19.200000000000003</v>
       </c>
+      <c r="F12" s="3">
+        <f>B12/19</f>
+        <v>18.789473684210527</v>
+      </c>
+      <c r="G12" s="4">
+        <f>C12/19</f>
+        <v>1.5631578947368421</v>
+      </c>
     </row>
     <row r="13" ht="14.25">
-      <c r="A13" s="3">
+      <c r="A13" s="6">
         <v>11</v>
       </c>
-      <c r="B13" s="3">
-        <f>$G$2+$I$2+($G$2-B2)</f>
+      <c r="B13" s="6">
+        <f>$H$2+$J$2+($H$2-B2)</f>
         <v>378.39999999999998</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="6">
         <v>30.899999999999999</v>
       </c>
-      <c r="D13" s="3">
-        <f>ROUND(B13/$G$2*224,1)-1</f>
+      <c r="D13">
+        <f>MAX(0,ROUND(B13/$H$2*224,1)-1)</f>
         <v>607.89999999999998</v>
       </c>
-      <c r="E13" s="1">
-        <f>ROUND(C13/$H$2*64,1)-1</f>
+      <c r="E13" s="2">
+        <f>MAX(0,ROUND(C13/$I$2*64,1)-1)</f>
         <v>20</v>
       </c>
+      <c r="F13" s="3">
+        <f>B13/19</f>
+        <v>19.91578947368421</v>
+      </c>
+      <c r="G13" s="4">
+        <f>C13/19</f>
+        <v>1.6263157894736842</v>
+      </c>
     </row>
     <row r="14" ht="14.25">
-      <c r="A14" s="2">
+      <c r="A14" s="5">
         <v>12</v>
       </c>
       <c r="B14">
@@ -891,16 +1008,24 @@
         <v>49.799999999999997</v>
       </c>
       <c r="D14">
-        <f>ROUND(B14/$G$2*224,1)-1</f>
+        <f>MAX(0,ROUND(B14/$H$2*224,1)-1)</f>
         <v>1.6000000000000001</v>
       </c>
-      <c r="E14" s="1">
-        <f>ROUND(C14/$H$2*64,1)-1</f>
+      <c r="E14" s="2">
+        <f>MAX(0,ROUND(C14/$I$2*64,1)-1)</f>
         <v>32.800000000000004</v>
       </c>
+      <c r="F14" s="3">
+        <f>B14/19</f>
+        <v>0.084210526315789472</v>
+      </c>
+      <c r="G14" s="4">
+        <f>C14/19</f>
+        <v>2.6210526315789471</v>
+      </c>
     </row>
     <row r="15" ht="14.25">
-      <c r="A15" s="2">
+      <c r="A15" s="5">
         <v>13</v>
       </c>
       <c r="B15">
@@ -910,16 +1035,24 @@
         <v>48.700000000000003</v>
       </c>
       <c r="D15">
-        <f>ROUND(B15/$G$2*224,1)-1</f>
+        <f>MAX(0,ROUND(B15/$H$2*224,1)-1)</f>
         <v>34.600000000000001</v>
       </c>
-      <c r="E15" s="1">
-        <f>ROUND(C15/$H$2*64,1)-1</f>
+      <c r="E15" s="2">
+        <f>MAX(0,ROUND(C15/$I$2*64,1)-1)</f>
         <v>32.100000000000001</v>
       </c>
+      <c r="F15" s="3">
+        <f>B15/19</f>
+        <v>1.1631578947368422</v>
+      </c>
+      <c r="G15" s="4">
+        <f>C15/19</f>
+        <v>2.5631578947368423</v>
+      </c>
     </row>
     <row r="16" ht="14.25">
-      <c r="A16" s="2">
+      <c r="A16" s="5">
         <v>14</v>
       </c>
       <c r="B16">
@@ -929,16 +1062,24 @@
         <v>28.600000000000001</v>
       </c>
       <c r="D16">
-        <f>ROUND(B16/$G$2*224,1)-1</f>
+        <f>MAX(0,ROUND(B16/$H$2*224,1)-1)</f>
         <v>67.100000000000009</v>
       </c>
-      <c r="E16" s="1">
-        <f>ROUND(C16/$H$2*64,1)-1</f>
+      <c r="E16" s="2">
+        <f>MAX(0,ROUND(C16/$I$2*64,1)-1)</f>
         <v>18.400000000000002</v>
       </c>
+      <c r="F16" s="3">
+        <f>B16/19</f>
+        <v>2.2263157894736842</v>
+      </c>
+      <c r="G16" s="4">
+        <f>C16/19</f>
+        <v>1.5052631578947369</v>
+      </c>
     </row>
     <row r="17" ht="14.25">
-      <c r="A17" s="2">
+      <c r="A17" s="5">
         <v>15</v>
       </c>
       <c r="B17">
@@ -948,16 +1089,24 @@
         <v>19</v>
       </c>
       <c r="D17">
-        <f>ROUND(B17/$G$2*224,1)-1</f>
+        <f>MAX(0,ROUND(B17/$H$2*224,1)-1)</f>
         <v>99.100000000000009</v>
       </c>
-      <c r="E17" s="1">
-        <f>ROUND(C17/$H$2*64,1)-1</f>
+      <c r="E17" s="2">
+        <f>MAX(0,ROUND(C17/$I$2*64,1)-1)</f>
         <v>11.9</v>
       </c>
+      <c r="F17" s="3">
+        <f>B17/19</f>
+        <v>3.2736842105263158</v>
+      </c>
+      <c r="G17" s="4">
+        <f>C17/19</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="18" ht="14.25">
-      <c r="A18" s="2">
+      <c r="A18" s="5">
         <v>16</v>
       </c>
       <c r="B18">
@@ -967,16 +1116,24 @@
         <v>35</v>
       </c>
       <c r="D18">
-        <f>ROUND(B18/$G$2*224,1)-1</f>
+        <f>MAX(0,ROUND(B18/$H$2*224,1)-1)</f>
         <v>129.30000000000001</v>
       </c>
-      <c r="E18" s="1">
-        <f>ROUND(C18/$H$2*64,1)-1</f>
+      <c r="E18" s="2">
+        <f>MAX(0,ROUND(C18/$I$2*64,1)-1)</f>
         <v>22.800000000000001</v>
       </c>
+      <c r="F18" s="3">
+        <f>B18/19</f>
+        <v>4.2631578947368425</v>
+      </c>
+      <c r="G18" s="4">
+        <f>C18/19</f>
+        <v>1.8421052631578947</v>
+      </c>
     </row>
     <row r="19" ht="14.25">
-      <c r="A19" s="2">
+      <c r="A19" s="5">
         <v>17</v>
       </c>
       <c r="B19">
@@ -986,136 +1143,192 @@
         <v>36.799999999999997</v>
       </c>
       <c r="D19">
-        <f>ROUND(B19/$G$2*224,1)-1</f>
+        <f>MAX(0,ROUND(B19/$H$2*224,1)-1)</f>
         <v>162.30000000000001</v>
       </c>
-      <c r="E19" s="1">
-        <f>ROUND(C19/$H$2*64,1)-1</f>
+      <c r="E19" s="2">
+        <f>MAX(0,ROUND(C19/$I$2*64,1)-1)</f>
         <v>24</v>
       </c>
+      <c r="F19" s="3">
+        <f>B19/19</f>
+        <v>5.3421052631578947</v>
+      </c>
+      <c r="G19" s="4">
+        <f>C19/19</f>
+        <v>1.9368421052631577</v>
+      </c>
     </row>
     <row r="20" ht="14.25">
-      <c r="A20" s="3">
+      <c r="A20" s="6">
         <v>18</v>
       </c>
-      <c r="B20" s="3">
-        <f>$G$2+$I$2+($G$2-B19)</f>
+      <c r="B20" s="6">
+        <f>$H$2+$J$2+($H$2-B19)</f>
         <v>276.89999999999998</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="6">
         <v>36.799999999999997</v>
       </c>
-      <c r="D20" s="3">
-        <f>ROUND(B20/$G$2*224,1)-1</f>
+      <c r="D20">
+        <f>MAX(0,ROUND(B20/$H$2*224,1)-1)</f>
         <v>444.60000000000002</v>
       </c>
-      <c r="E20" s="1">
-        <f>ROUND(C20/$H$2*64,1)-1</f>
+      <c r="E20" s="2">
+        <f>MAX(0,ROUND(C20/$I$2*64,1)-1)</f>
         <v>24</v>
       </c>
+      <c r="F20" s="3">
+        <f>B20/19</f>
+        <v>14.573684210526315</v>
+      </c>
+      <c r="G20" s="4">
+        <f>C20/19</f>
+        <v>1.9368421052631577</v>
+      </c>
     </row>
     <row r="21" ht="14.25">
-      <c r="A21" s="3">
+      <c r="A21" s="6">
         <v>19</v>
       </c>
-      <c r="B21" s="3">
-        <f>$G$2+$I$2+($G$2-B18)</f>
+      <c r="B21" s="6">
+        <f>$H$2+$J$2+($H$2-B18)</f>
         <v>297.39999999999998</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="6">
         <v>35</v>
       </c>
-      <c r="D21" s="3">
-        <f>ROUND(B21/$G$2*224,1)-1</f>
+      <c r="D21">
+        <f>MAX(0,ROUND(B21/$H$2*224,1)-1)</f>
         <v>477.60000000000002</v>
       </c>
-      <c r="E21" s="1">
-        <f>ROUND(C21/$H$2*64,1)-1</f>
+      <c r="E21" s="2">
+        <f>MAX(0,ROUND(C21/$I$2*64,1)-1)</f>
         <v>22.800000000000001</v>
       </c>
+      <c r="F21" s="3">
+        <f>B21/19</f>
+        <v>15.652631578947368</v>
+      </c>
+      <c r="G21" s="4">
+        <f>C21/19</f>
+        <v>1.8421052631578947</v>
+      </c>
     </row>
     <row r="22" ht="14.25">
-      <c r="A22" s="3">
+      <c r="A22" s="6">
         <v>20</v>
       </c>
-      <c r="B22" s="3">
-        <f>$G$2+$I$2+($G$2-B17)</f>
+      <c r="B22" s="6">
+        <f>$H$2+$J$2+($H$2-B17)</f>
         <v>316.19999999999999</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="6">
         <v>19</v>
       </c>
-      <c r="D22" s="3">
-        <f>ROUND(B22/$G$2*224,1)-1</f>
+      <c r="D22">
+        <f>MAX(0,ROUND(B22/$H$2*224,1)-1)</f>
         <v>507.80000000000001</v>
       </c>
-      <c r="E22" s="1">
-        <f>ROUND(C22/$H$2*64,1)-1</f>
+      <c r="E22" s="2">
+        <f>MAX(0,ROUND(C22/$I$2*64,1)-1)</f>
         <v>11.9</v>
       </c>
+      <c r="F22" s="3">
+        <f>B22/19</f>
+        <v>16.642105263157895</v>
+      </c>
+      <c r="G22" s="4">
+        <f>C22/19</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="23" ht="14.25">
-      <c r="A23" s="3">
+      <c r="A23" s="6">
         <v>21</v>
       </c>
-      <c r="B23" s="3">
-        <f>$G$2+$I$2+($G$2-B16)</f>
+      <c r="B23" s="6">
+        <f>$H$2+$J$2+($H$2-B16)</f>
         <v>336.09999999999997</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="6">
         <v>28.600000000000001</v>
       </c>
-      <c r="D23" s="3">
-        <f>ROUND(B23/$G$2*224,1)-1</f>
+      <c r="D23">
+        <f>MAX(0,ROUND(B23/$H$2*224,1)-1)</f>
         <v>539.89999999999998</v>
       </c>
-      <c r="E23" s="1">
-        <f>ROUND(C23/$H$2*64,1)-1</f>
+      <c r="E23" s="2">
+        <f>MAX(0,ROUND(C23/$I$2*64,1)-1)</f>
         <v>18.400000000000002</v>
       </c>
+      <c r="F23" s="3">
+        <f>B23/19</f>
+        <v>17.689473684210526</v>
+      </c>
+      <c r="G23" s="4">
+        <f>C23/19</f>
+        <v>1.5052631578947369</v>
+      </c>
     </row>
     <row r="24" ht="14.25">
-      <c r="A24" s="3">
+      <c r="A24" s="6">
         <v>22</v>
       </c>
-      <c r="B24" s="3">
-        <f>$G$2+$I$2+($G$2-B15)</f>
+      <c r="B24" s="6">
+        <f>$H$2+$J$2+($H$2-B15)</f>
         <v>356.29999999999995</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="6">
         <v>48.700000000000003</v>
       </c>
-      <c r="D24" s="3">
-        <f>ROUND(B24/$G$2*224,1)-1</f>
+      <c r="D24">
+        <f>MAX(0,ROUND(B24/$H$2*224,1)-1)</f>
         <v>572.39999999999998</v>
       </c>
-      <c r="E24" s="1">
-        <f>ROUND(C24/$H$2*64,1)-1</f>
+      <c r="E24" s="2">
+        <f>MAX(0,ROUND(C24/$I$2*64,1)-1)</f>
         <v>32.100000000000001</v>
       </c>
+      <c r="F24" s="3">
+        <f>B24/19</f>
+        <v>18.752631578947366</v>
+      </c>
+      <c r="G24" s="4">
+        <f>C24/19</f>
+        <v>2.5631578947368423</v>
+      </c>
     </row>
     <row r="25" ht="14.25">
-      <c r="A25" s="3">
+      <c r="A25" s="6">
         <v>23</v>
       </c>
-      <c r="B25" s="3">
-        <f>$G$2+$I$2+($G$2-B14)</f>
+      <c r="B25" s="6">
+        <f>$H$2+$J$2+($H$2-B14)</f>
         <v>376.79999999999995</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="6">
         <v>49.799999999999997</v>
       </c>
-      <c r="D25" s="3">
-        <f>ROUND(B25/$G$2*224,1)-1</f>
+      <c r="D25">
+        <f>MAX(0,ROUND(B25/$H$2*224,1)-1)</f>
         <v>605.30000000000007</v>
       </c>
-      <c r="E25" s="1">
-        <f>ROUND(C25/$H$2*64,1)-1</f>
+      <c r="E25" s="2">
+        <f>MAX(0,ROUND(C25/$I$2*64,1)-1)</f>
         <v>32.800000000000004</v>
       </c>
+      <c r="F25" s="3">
+        <f>B25/19</f>
+        <v>19.831578947368417</v>
+      </c>
+      <c r="G25" s="4">
+        <f>C25/19</f>
+        <v>2.6210526315789471</v>
+      </c>
     </row>
     <row r="26" ht="14.25">
-      <c r="A26" s="2">
+      <c r="A26" s="5">
         <v>24</v>
       </c>
       <c r="B26">
@@ -1125,16 +1338,24 @@
         <v>68.700000000000003</v>
       </c>
       <c r="D26">
-        <f>ROUND(B26/$G$2*224,1)-1</f>
+        <f>MAX(0,ROUND(B26/$H$2*224,1)-1)</f>
         <v>4.3000000000000007</v>
       </c>
-      <c r="E26" s="1">
-        <f>ROUND(C26/$H$2*64,1)-1</f>
+      <c r="E26" s="2">
+        <f>MAX(0,ROUND(C26/$I$2*64,1)-1)</f>
         <v>45.700000000000003</v>
       </c>
+      <c r="F26" s="3">
+        <f>B26/19</f>
+        <v>0.17368421052631577</v>
+      </c>
+      <c r="G26" s="4">
+        <f>C26/19</f>
+        <v>3.6157894736842109</v>
+      </c>
     </row>
     <row r="27" ht="14.25">
-      <c r="A27" s="2">
+      <c r="A27" s="5">
         <v>25</v>
       </c>
       <c r="B27">
@@ -1144,16 +1365,24 @@
         <v>67.599999999999994</v>
       </c>
       <c r="D27">
-        <f>ROUND(B27/$G$2*224,1)-1</f>
+        <f>MAX(0,ROUND(B27/$H$2*224,1)-1)</f>
         <v>35.600000000000001</v>
       </c>
-      <c r="E27" s="1">
-        <f>ROUND(C27/$H$2*64,1)-1</f>
+      <c r="E27" s="2">
+        <f>MAX(0,ROUND(C27/$I$2*64,1)-1)</f>
         <v>44.900000000000006</v>
       </c>
+      <c r="F27" s="3">
+        <f>B27/19</f>
+        <v>1.1973684210526316</v>
+      </c>
+      <c r="G27" s="4">
+        <f>C27/19</f>
+        <v>3.5578947368421048</v>
+      </c>
     </row>
     <row r="28" ht="14.25">
-      <c r="A28" s="2">
+      <c r="A28" s="5">
         <v>26</v>
       </c>
       <c r="B28">
@@ -1163,16 +1392,24 @@
         <v>47.600000000000001</v>
       </c>
       <c r="D28">
-        <f>ROUND(B28/$G$2*224,1)-1</f>
+        <f>MAX(0,ROUND(B28/$H$2*224,1)-1)</f>
         <v>66.600000000000009</v>
       </c>
-      <c r="E28" s="1">
-        <f>ROUND(C28/$H$2*64,1)-1</f>
+      <c r="E28" s="2">
+        <f>MAX(0,ROUND(C28/$I$2*64,1)-1)</f>
         <v>31.300000000000004</v>
       </c>
+      <c r="F28" s="3">
+        <f>B28/19</f>
+        <v>2.2105263157894739</v>
+      </c>
+      <c r="G28" s="4">
+        <f>C28/19</f>
+        <v>2.5052631578947371</v>
+      </c>
     </row>
     <row r="29" ht="14.25">
-      <c r="A29" s="2">
+      <c r="A29" s="5">
         <v>27</v>
       </c>
       <c r="B29">
@@ -1182,16 +1419,24 @@
         <v>38</v>
       </c>
       <c r="D29">
-        <f>ROUND(B29/$G$2*224,1)-1</f>
+        <f>MAX(0,ROUND(B29/$H$2*224,1)-1)</f>
         <v>97.5</v>
       </c>
-      <c r="E29" s="1">
-        <f>ROUND(C29/$H$2*64,1)-1</f>
+      <c r="E29" s="2">
+        <f>MAX(0,ROUND(C29/$I$2*64,1)-1)</f>
         <v>24.800000000000001</v>
       </c>
+      <c r="F29" s="3">
+        <f>B29/19</f>
+        <v>3.2210526315789476</v>
+      </c>
+      <c r="G29" s="4">
+        <f>C29/19</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="30" ht="14.25">
-      <c r="A30" s="2">
+      <c r="A30" s="5">
         <v>28</v>
       </c>
       <c r="B30">
@@ -1201,16 +1446,24 @@
         <v>53.899999999999999</v>
       </c>
       <c r="D30">
-        <f>ROUND(B30/$G$2*224,1)-1</f>
+        <f>MAX(0,ROUND(B30/$H$2*224,1)-1)</f>
         <v>126.80000000000001</v>
       </c>
-      <c r="E30" s="1">
-        <f>ROUND(C30/$H$2*64,1)-1</f>
+      <c r="E30" s="2">
+        <f>MAX(0,ROUND(C30/$I$2*64,1)-1)</f>
         <v>35.600000000000001</v>
       </c>
+      <c r="F30" s="3">
+        <f>B30/19</f>
+        <v>4.1789473684210527</v>
+      </c>
+      <c r="G30" s="4">
+        <f>C30/19</f>
+        <v>2.8368421052631576</v>
+      </c>
     </row>
     <row r="31" ht="14.25">
-      <c r="A31" s="2">
+      <c r="A31" s="5">
         <v>29</v>
       </c>
       <c r="B31">
@@ -1220,136 +1473,192 @@
         <v>55.600000000000001</v>
       </c>
       <c r="D31">
-        <f>ROUND(B31/$G$2*224,1)-1</f>
+        <f>MAX(0,ROUND(B31/$H$2*224,1)-1)</f>
         <v>158.10000000000002</v>
       </c>
-      <c r="E31" s="1">
-        <f>ROUND(C31/$H$2*64,1)-1</f>
+      <c r="E31" s="2">
+        <f>MAX(0,ROUND(C31/$I$2*64,1)-1)</f>
         <v>36.800000000000004</v>
       </c>
+      <c r="F31" s="3">
+        <f>B31/19</f>
+        <v>5.2052631578947368</v>
+      </c>
+      <c r="G31" s="4">
+        <f>C31/19</f>
+        <v>2.9263157894736844</v>
+      </c>
     </row>
     <row r="32" ht="14.25">
-      <c r="A32" s="3">
+      <c r="A32" s="6">
         <v>30</v>
       </c>
-      <c r="B32" s="3">
-        <f>$G$2+$I$2+($G$2-B31)</f>
+      <c r="B32" s="6">
+        <f>$H$2+$J$2+($H$2-B31)</f>
         <v>279.5</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32" s="6">
         <v>55.600000000000001</v>
       </c>
-      <c r="D32" s="3">
-        <f>ROUND(B32/$G$2*224,1)-1</f>
+      <c r="D32">
+        <f>MAX(0,ROUND(B32/$H$2*224,1)-1)</f>
         <v>448.80000000000001</v>
       </c>
-      <c r="E32" s="1">
-        <f>ROUND(C32/$H$2*64,1)-1</f>
+      <c r="E32" s="2">
+        <f>MAX(0,ROUND(C32/$I$2*64,1)-1)</f>
         <v>36.800000000000004</v>
       </c>
+      <c r="F32" s="3">
+        <f>B32/19</f>
+        <v>14.710526315789474</v>
+      </c>
+      <c r="G32" s="4">
+        <f>C32/19</f>
+        <v>2.9263157894736844</v>
+      </c>
     </row>
     <row r="33" ht="14.25">
-      <c r="A33" s="3">
+      <c r="A33" s="6">
         <v>31</v>
       </c>
-      <c r="B33" s="3">
-        <f>$G$2+$I$2+($G$2-B30)</f>
+      <c r="B33" s="6">
+        <f>$H$2+$J$2+($H$2-B30)</f>
         <v>299</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C33" s="6">
         <v>53.899999999999999</v>
       </c>
-      <c r="D33" s="3">
-        <f>ROUND(B33/$G$2*224,1)-1</f>
+      <c r="D33">
+        <f>MAX(0,ROUND(B33/$H$2*224,1)-1)</f>
         <v>480.10000000000002</v>
       </c>
-      <c r="E33" s="1">
-        <f>ROUND(C33/$H$2*64,1)-1</f>
+      <c r="E33" s="2">
+        <f>MAX(0,ROUND(C33/$I$2*64,1)-1)</f>
         <v>35.600000000000001</v>
       </c>
+      <c r="F33" s="3">
+        <f>B33/19</f>
+        <v>15.736842105263158</v>
+      </c>
+      <c r="G33" s="4">
+        <f>C33/19</f>
+        <v>2.8368421052631576</v>
+      </c>
     </row>
     <row r="34" ht="14.25">
-      <c r="A34" s="3">
+      <c r="A34" s="6">
         <v>32</v>
       </c>
-      <c r="B34" s="3">
-        <f>$G$2+$I$2+($G$2-B29)</f>
+      <c r="B34" s="6">
+        <f>$H$2+$J$2+($H$2-B29)</f>
         <v>317.19999999999999</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34" s="6">
         <v>38</v>
       </c>
-      <c r="D34" s="3">
-        <f>ROUND(B34/$G$2*224,1)-1</f>
+      <c r="D34">
+        <f>MAX(0,ROUND(B34/$H$2*224,1)-1)</f>
         <v>509.40000000000003</v>
       </c>
-      <c r="E34" s="1">
-        <f>ROUND(C34/$H$2*64,1)-1</f>
+      <c r="E34" s="2">
+        <f>MAX(0,ROUND(C34/$I$2*64,1)-1)</f>
         <v>24.800000000000001</v>
       </c>
+      <c r="F34" s="3">
+        <f>B34/19</f>
+        <v>16.694736842105261</v>
+      </c>
+      <c r="G34" s="4">
+        <f>C34/19</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="35" ht="14.25">
-      <c r="A35" s="3">
+      <c r="A35" s="6">
         <v>33</v>
       </c>
-      <c r="B35" s="3">
-        <f>$G$2+$I$2+($G$2-B28)</f>
+      <c r="B35" s="6">
+        <f>$H$2+$J$2+($H$2-B28)</f>
         <v>336.39999999999998</v>
       </c>
-      <c r="C35" s="3">
+      <c r="C35" s="6">
         <v>47.600000000000001</v>
       </c>
-      <c r="D35" s="3">
-        <f>ROUND(B35/$G$2*224,1)-1</f>
+      <c r="D35">
+        <f>MAX(0,ROUND(B35/$H$2*224,1)-1)</f>
         <v>540.30000000000007</v>
       </c>
-      <c r="E35" s="1">
-        <f>ROUND(C35/$H$2*64,1)-1</f>
+      <c r="E35" s="2">
+        <f>MAX(0,ROUND(C35/$I$2*64,1)-1)</f>
         <v>31.300000000000004</v>
       </c>
+      <c r="F35" s="3">
+        <f>B35/19</f>
+        <v>17.705263157894734</v>
+      </c>
+      <c r="G35" s="4">
+        <f>C35/19</f>
+        <v>2.5052631578947371</v>
+      </c>
     </row>
     <row r="36" ht="14.25">
-      <c r="A36" s="3">
+      <c r="A36" s="6">
         <v>34</v>
       </c>
-      <c r="B36" s="3">
-        <f>$G$2+$I$2+($G$2-B27)</f>
+      <c r="B36" s="6">
+        <f>$H$2+$J$2+($H$2-B27)</f>
         <v>355.64999999999998</v>
       </c>
-      <c r="C36" s="3">
+      <c r="C36" s="6">
         <v>67.599999999999994</v>
       </c>
-      <c r="D36" s="3">
-        <f>ROUND(B36/$G$2*224,1)-1</f>
+      <c r="D36">
+        <f>MAX(0,ROUND(B36/$H$2*224,1)-1)</f>
         <v>571.30000000000007</v>
       </c>
-      <c r="E36" s="1">
-        <f>ROUND(C36/$H$2*64,1)-1</f>
+      <c r="E36" s="2">
+        <f>MAX(0,ROUND(C36/$I$2*64,1)-1)</f>
         <v>44.900000000000006</v>
       </c>
+      <c r="F36" s="3">
+        <f>B36/19</f>
+        <v>18.718421052631577</v>
+      </c>
+      <c r="G36" s="4">
+        <f>C36/19</f>
+        <v>3.5578947368421048</v>
+      </c>
     </row>
     <row r="37" ht="14.25">
-      <c r="A37" s="3">
+      <c r="A37" s="6">
         <v>35</v>
       </c>
-      <c r="B37" s="3">
-        <f>$G$2+$I$2+($G$2-B26)</f>
+      <c r="B37" s="6">
+        <f>$H$2+$J$2+($H$2-B26)</f>
         <v>375.09999999999997</v>
       </c>
-      <c r="C37" s="3">
+      <c r="C37" s="6">
         <v>68.700000000000003</v>
       </c>
-      <c r="D37" s="3">
-        <f>ROUND(B37/$G$2*224,1)-1</f>
+      <c r="D37">
+        <f>MAX(0,ROUND(B37/$H$2*224,1)-1)</f>
         <v>602.60000000000002</v>
       </c>
-      <c r="E37" s="1">
-        <f>ROUND(C37/$H$2*64,1)-1</f>
+      <c r="E37" s="2">
+        <f>MAX(0,ROUND(C37/$I$2*64,1)-1)</f>
         <v>45.700000000000003</v>
       </c>
+      <c r="F37" s="3">
+        <f>B37/19</f>
+        <v>19.742105263157892</v>
+      </c>
+      <c r="G37" s="4">
+        <f>C37/19</f>
+        <v>3.6157894736842109</v>
+      </c>
     </row>
     <row r="38" ht="14.25">
-      <c r="A38" s="2">
+      <c r="A38" s="5">
         <v>36</v>
       </c>
       <c r="B38">
@@ -1359,16 +1668,24 @@
         <v>73.900000000000006</v>
       </c>
       <c r="D38">
-        <f>ROUND(B38/$G$2*224,1)-1</f>
+        <f>MAX(0,ROUND(B38/$H$2*224,1)-1)</f>
         <v>95.100000000000009</v>
       </c>
-      <c r="E38" s="1">
-        <f>ROUND(C38/$H$2*64,1)-1</f>
+      <c r="E38" s="2">
+        <f>MAX(0,ROUND(C38/$I$2*64,1)-1)</f>
         <v>49.200000000000003</v>
       </c>
+      <c r="F38" s="3">
+        <f>B38/19</f>
+        <v>3.142105263157895</v>
+      </c>
+      <c r="G38" s="4">
+        <f>C38/19</f>
+        <v>3.8894736842105266</v>
+      </c>
     </row>
     <row r="39" ht="14.25">
-      <c r="A39" s="2">
+      <c r="A39" s="5">
         <v>37</v>
       </c>
       <c r="B39">
@@ -1378,56 +1695,80 @@
         <v>75.200000000000003</v>
       </c>
       <c r="D39">
-        <f>ROUND(B39/$G$2*224,1)-1</f>
+        <f>MAX(0,ROUND(B39/$H$2*224,1)-1)</f>
         <v>125.5</v>
       </c>
-      <c r="E39" s="1">
-        <f>ROUND(C39/$H$2*64,1)-1</f>
+      <c r="E39" s="2">
+        <f>MAX(0,ROUND(C39/$I$2*64,1)-1)</f>
         <v>50.100000000000001</v>
       </c>
+      <c r="F39" s="3">
+        <f>B39/19</f>
+        <v>4.1368421052631579</v>
+      </c>
+      <c r="G39" s="4">
+        <f>C39/19</f>
+        <v>3.9578947368421056</v>
+      </c>
     </row>
     <row r="40" ht="14.25">
-      <c r="A40" s="3">
+      <c r="A40" s="6">
         <v>38</v>
       </c>
-      <c r="B40" s="3">
-        <f>$G$2+$I$2+($G$2-B39)</f>
+      <c r="B40" s="6">
+        <f>$H$2+$J$2+($H$2-B39)</f>
         <v>299.79999999999995</v>
       </c>
-      <c r="C40" s="3">
+      <c r="C40" s="6">
         <v>75.200000000000003</v>
       </c>
-      <c r="D40" s="3">
-        <f>ROUND(B40/$G$2*224,1)-1</f>
+      <c r="D40">
+        <f>MAX(0,ROUND(B40/$H$2*224,1)-1)</f>
         <v>481.40000000000003</v>
       </c>
-      <c r="E40" s="1">
-        <f>ROUND(C40/$H$2*64,1)-1</f>
+      <c r="E40" s="2">
+        <f>MAX(0,ROUND(C40/$I$2*64,1)-1)</f>
         <v>50.100000000000001</v>
       </c>
+      <c r="F40" s="3">
+        <f>B40/19</f>
+        <v>15.778947368421051</v>
+      </c>
+      <c r="G40" s="4">
+        <f>C40/19</f>
+        <v>3.9578947368421056</v>
+      </c>
     </row>
     <row r="41" ht="14.25">
-      <c r="A41" s="3">
+      <c r="A41" s="6">
         <v>39</v>
       </c>
-      <c r="B41" s="3">
-        <f>$G$2+$I$2+($G$2-B38)</f>
+      <c r="B41" s="6">
+        <f>$H$2+$J$2+($H$2-B38)</f>
         <v>318.69999999999999</v>
       </c>
-      <c r="C41" s="3">
+      <c r="C41" s="6">
         <v>73.900000000000006</v>
       </c>
-      <c r="D41" s="3">
-        <f>ROUND(B41/$G$2*224,1)-1</f>
+      <c r="D41">
+        <f>MAX(0,ROUND(B41/$H$2*224,1)-1)</f>
         <v>511.89999999999998</v>
       </c>
-      <c r="E41" s="1">
-        <f>ROUND(C41/$H$2*64,1)-1</f>
+      <c r="E41" s="2">
+        <f>MAX(0,ROUND(C41/$I$2*64,1)-1)</f>
         <v>49.200000000000003</v>
       </c>
+      <c r="F41" s="3">
+        <f>B41/19</f>
+        <v>16.773684210526316</v>
+      </c>
+      <c r="G41" s="4">
+        <f>C41/19</f>
+        <v>3.8894736842105266</v>
+      </c>
     </row>
     <row r="42" ht="14.25">
-      <c r="A42" s="2">
+      <c r="A42" s="5">
         <v>40</v>
       </c>
       <c r="B42">
@@ -1437,16 +1778,24 @@
         <v>92.900000000000006</v>
       </c>
       <c r="D42">
-        <f>ROUND(B42/$G$2*224,1)-1</f>
+        <f>MAX(0,ROUND(B42/$H$2*224,1)-1)</f>
         <v>92.800000000000011</v>
       </c>
-      <c r="E42" s="1">
-        <f>ROUND(C42/$H$2*64,1)-1</f>
+      <c r="E42" s="2">
+        <f>MAX(0,ROUND(C42/$I$2*64,1)-1)</f>
         <v>62.100000000000001</v>
       </c>
+      <c r="F42" s="3">
+        <f>B42/19</f>
+        <v>3.0684210526315789</v>
+      </c>
+      <c r="G42" s="4">
+        <f>C42/19</f>
+        <v>4.8894736842105262</v>
+      </c>
     </row>
     <row r="43" ht="14.25">
-      <c r="A43" s="2">
+      <c r="A43" s="5">
         <v>41</v>
       </c>
       <c r="B43">
@@ -1456,16 +1805,24 @@
         <v>94.200000000000003</v>
       </c>
       <c r="D43">
-        <f>ROUND(B43/$G$2*224,1)-1</f>
+        <f>MAX(0,ROUND(B43/$H$2*224,1)-1)</f>
         <v>123.40000000000001</v>
       </c>
-      <c r="E43" s="1">
-        <f>ROUND(C43/$H$2*64,1)-1</f>
+      <c r="E43" s="2">
+        <f>MAX(0,ROUND(C43/$I$2*64,1)-1)</f>
         <v>63</v>
       </c>
+      <c r="F43" s="3">
+        <f>B43/19</f>
+        <v>4.0684210526315789</v>
+      </c>
+      <c r="G43" s="4">
+        <f>C43/19</f>
+        <v>4.9578947368421051</v>
+      </c>
     </row>
     <row r="44" ht="14.25">
-      <c r="A44" s="2">
+      <c r="A44" s="5">
         <v>42</v>
       </c>
       <c r="B44">
@@ -1475,16 +1832,24 @@
         <v>86</v>
       </c>
       <c r="D44">
-        <f>ROUND(B44/$G$2*224,1)-1</f>
+        <f>MAX(0,ROUND(B44/$H$2*224,1)-1)</f>
         <v>154.90000000000001</v>
       </c>
-      <c r="E44" s="1">
-        <f>ROUND(C44/$H$2*64,1)-1</f>
+      <c r="E44" s="2">
+        <f>MAX(0,ROUND(C44/$I$2*64,1)-1)</f>
         <v>57.400000000000006</v>
       </c>
+      <c r="F44" s="3">
+        <f>B44/19</f>
+        <v>5.1000000000000005</v>
+      </c>
+      <c r="G44" s="4">
+        <f>C44/19</f>
+        <v>4.5263157894736841</v>
+      </c>
     </row>
     <row r="45" ht="14.25">
-      <c r="A45" s="2">
+      <c r="A45" s="5">
         <v>43</v>
       </c>
       <c r="B45">
@@ -1494,16 +1859,24 @@
         <v>88.599999999999994</v>
       </c>
       <c r="D45">
-        <f>ROUND(B45/$G$2*224,1)-1</f>
+        <f>MAX(0,ROUND(B45/$H$2*224,1)-1)</f>
         <v>187.40000000000001</v>
       </c>
-      <c r="E45" s="1">
-        <f>ROUND(C45/$H$2*64,1)-1</f>
+      <c r="E45" s="2">
+        <f>MAX(0,ROUND(C45/$I$2*64,1)-1)</f>
         <v>59.200000000000003</v>
       </c>
+      <c r="F45" s="3">
+        <f>B45/19</f>
+        <v>6.1631578947368419</v>
+      </c>
+      <c r="G45" s="4">
+        <f>C45/19</f>
+        <v>4.6631578947368419</v>
+      </c>
     </row>
     <row r="46" ht="14.25">
-      <c r="A46" s="2">
+      <c r="A46" s="5">
         <v>44</v>
       </c>
       <c r="B46">
@@ -1513,112 +1886,160 @@
         <v>89.700000000000003</v>
       </c>
       <c r="D46">
-        <f>ROUND(B46/$G$2*224,1)-1</f>
+        <f>MAX(0,ROUND(B46/$H$2*224,1)-1)</f>
         <v>223</v>
       </c>
-      <c r="E46" s="1">
-        <f>ROUND(C46/$H$2*64,1)-1</f>
+      <c r="E46" s="2">
+        <f>MAX(0,ROUND(C46/$I$2*64,1)-1)</f>
         <v>59.900000000000006</v>
       </c>
+      <c r="F46" s="3">
+        <f>B46/19</f>
+        <v>7.3263157894736839</v>
+      </c>
+      <c r="G46" s="4">
+        <f>C46/19</f>
+        <v>4.7210526315789476</v>
+      </c>
     </row>
     <row r="47" ht="14.25">
-      <c r="A47" s="3">
+      <c r="A47" s="6">
         <v>45</v>
       </c>
-      <c r="B47" s="3">
-        <f>$G$2+$I$2+($G$2-B46)</f>
+      <c r="B47" s="6">
+        <f>$H$2+$J$2+($H$2-B46)</f>
         <v>239.19999999999999</v>
       </c>
-      <c r="C47" s="3">
+      <c r="C47" s="6">
         <v>89.700000000000003</v>
       </c>
-      <c r="D47" s="3">
-        <f>ROUND(B47/$G$2*224,1)-1</f>
+      <c r="D47">
+        <f>MAX(0,ROUND(B47/$H$2*224,1)-1)</f>
         <v>383.90000000000003</v>
       </c>
-      <c r="E47" s="1">
-        <f>ROUND(C47/$H$2*64,1)-1</f>
+      <c r="E47" s="2">
+        <f>MAX(0,ROUND(C47/$I$2*64,1)-1)</f>
         <v>59.900000000000006</v>
       </c>
+      <c r="F47" s="3">
+        <f>B47/19</f>
+        <v>12.589473684210526</v>
+      </c>
+      <c r="G47" s="4">
+        <f>C47/19</f>
+        <v>4.7210526315789476</v>
+      </c>
     </row>
     <row r="48" ht="14.25">
-      <c r="A48" s="3">
+      <c r="A48" s="6">
         <v>46</v>
       </c>
-      <c r="B48" s="3">
-        <f>$G$2+$I$2+($G$2-B45)</f>
+      <c r="B48" s="6">
+        <f>$H$2+$J$2+($H$2-B45)</f>
         <v>261.29999999999995</v>
       </c>
-      <c r="C48" s="3">
+      <c r="C48" s="6">
         <v>88.599999999999994</v>
       </c>
-      <c r="D48" s="3">
-        <f>ROUND(B48/$G$2*224,1)-1</f>
+      <c r="D48">
+        <f>MAX(0,ROUND(B48/$H$2*224,1)-1)</f>
         <v>419.5</v>
       </c>
-      <c r="E48" s="1">
-        <f>ROUND(C48/$H$2*64,1)-1</f>
+      <c r="E48" s="2">
+        <f>MAX(0,ROUND(C48/$I$2*64,1)-1)</f>
         <v>59.200000000000003</v>
       </c>
+      <c r="F48" s="3">
+        <f>B48/19</f>
+        <v>13.752631578947366</v>
+      </c>
+      <c r="G48" s="4">
+        <f>C48/19</f>
+        <v>4.6631578947368419</v>
+      </c>
     </row>
     <row r="49" ht="14.25">
-      <c r="A49" s="3">
+      <c r="A49" s="6">
         <v>47</v>
       </c>
-      <c r="B49" s="3">
-        <f>$G$2+$I$2+($G$2-B44)</f>
+      <c r="B49" s="6">
+        <f>$H$2+$J$2+($H$2-B44)</f>
         <v>281.5</v>
       </c>
-      <c r="C49" s="3">
+      <c r="C49" s="6">
         <v>86</v>
       </c>
-      <c r="D49" s="3">
-        <f>ROUND(B49/$G$2*224,1)-1</f>
+      <c r="D49">
+        <f>MAX(0,ROUND(B49/$H$2*224,1)-1)</f>
         <v>452</v>
       </c>
-      <c r="E49" s="1">
-        <f>ROUND(C49/$H$2*64,1)-1</f>
+      <c r="E49" s="2">
+        <f>MAX(0,ROUND(C49/$I$2*64,1)-1)</f>
         <v>57.400000000000006</v>
       </c>
+      <c r="F49" s="3">
+        <f>B49/19</f>
+        <v>14.815789473684211</v>
+      </c>
+      <c r="G49" s="4">
+        <f>C49/19</f>
+        <v>4.5263157894736841</v>
+      </c>
     </row>
     <row r="50" ht="14.25">
-      <c r="A50" s="3">
+      <c r="A50" s="6">
         <v>48</v>
       </c>
-      <c r="B50" s="3">
-        <f>$G$2+$I$2+($G$2-B43)</f>
+      <c r="B50" s="6">
+        <f>$H$2+$J$2+($H$2-B43)</f>
         <v>301.09999999999997</v>
       </c>
-      <c r="C50" s="3">
+      <c r="C50" s="6">
         <v>94.200000000000003</v>
       </c>
-      <c r="D50" s="3">
-        <f>ROUND(B50/$G$2*224,1)-1</f>
+      <c r="D50">
+        <f>MAX(0,ROUND(B50/$H$2*224,1)-1)</f>
         <v>483.5</v>
       </c>
-      <c r="E50" s="1">
-        <f>ROUND(C50/$H$2*64,1)-1</f>
+      <c r="E50" s="2">
+        <f>MAX(0,ROUND(C50/$I$2*64,1)-1)</f>
         <v>63</v>
       </c>
+      <c r="F50" s="3">
+        <f>B50/19</f>
+        <v>15.84736842105263</v>
+      </c>
+      <c r="G50" s="4">
+        <f>C50/19</f>
+        <v>4.9578947368421051</v>
+      </c>
     </row>
     <row r="51" ht="14.25">
-      <c r="A51" s="3">
+      <c r="A51" s="6">
         <v>49</v>
       </c>
-      <c r="B51" s="3">
-        <f>$G$2+$I$2+($G$2-B42)</f>
+      <c r="B51" s="6">
+        <f>$H$2+$J$2+($H$2-B42)</f>
         <v>320.09999999999997</v>
       </c>
-      <c r="C51" s="3">
+      <c r="C51" s="6">
         <v>92.900000000000006</v>
       </c>
-      <c r="D51" s="3">
-        <f>ROUND(B51/$G$2*224,1)-1</f>
+      <c r="D51">
+        <f>MAX(0,ROUND(B51/$H$2*224,1)-1)</f>
         <v>514.10000000000002</v>
       </c>
-      <c r="E51" s="1">
-        <f>ROUND(C51/$H$2*64,1)-1</f>
+      <c r="E51" s="2">
+        <f>ROUND(C51/$I$2*64,1)-1</f>
         <v>62.100000000000001</v>
+      </c>
+      <c r="F51" s="3">
+        <f>B51/19</f>
+        <v>16.847368421052629</v>
+      </c>
+      <c r="G51" s="4">
+        <f>C51/19</f>
+        <v>4.8894736842105262</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Initial RGB matrix map
</commit_message>
<xml_diff>
--- a/firmware/key_physical_positions.xlsx
+++ b/firmware/key_physical_positions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>SW</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>X_BOARD_DIST</t>
+  </si>
+  <si>
+    <t>RGB_MAX_X</t>
   </si>
 </sst>
 </file>
@@ -93,14 +96,14 @@
   <cellXfs count="7">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="1" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="1" xfId="0" applyNumberFormat="1">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -624,6 +627,7 @@
     <col bestFit="1" min="4" max="4" width="8.7109375"/>
     <col bestFit="1" min="5" max="5" width="8.8515625"/>
     <col min="6" max="6" width="8.8515625"/>
+    <col bestFit="1" min="10" max="10" width="13.8515625"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
@@ -657,6 +661,9 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" ht="14.25">
       <c r="A2">
@@ -668,20 +675,20 @@
       <c r="C2">
         <v>30.899999999999999</v>
       </c>
-      <c r="D2">
-        <f>MAX(0,ROUND(B2/$H$2*224,1)-1)</f>
+      <c r="D2" s="2">
+        <f>MAX(0,ROUND(B2/$K$2*224,1)-1)</f>
         <v>0</v>
       </c>
-      <c r="E2" s="2">
-        <f>MAX(0,ROUND(C2/$I$2*64,1)-1)</f>
+      <c r="E2" s="3">
+        <f t="shared" ref="E2:E9" si="0">MAX(0,ROUND(C2/$I$2*64,1)-1)</f>
         <v>20</v>
       </c>
-      <c r="F2" s="3">
-        <f>B2/19</f>
+      <c r="F2" s="4">
+        <f t="shared" ref="F2:F9" si="1">B2/19</f>
         <v>0</v>
       </c>
-      <c r="G2" s="4">
-        <f>C2/19</f>
+      <c r="G2" s="5">
+        <f t="shared" ref="G2:G9" si="2">C2/19</f>
         <v>1.6263157894736842</v>
       </c>
       <c r="H2">
@@ -692,6 +699,10 @@
       </c>
       <c r="J2">
         <v>100</v>
+      </c>
+      <c r="K2">
+        <f>H2*2+J2</f>
+        <v>378.39999999999998</v>
       </c>
     </row>
     <row r="3" ht="14.25">
@@ -704,25 +715,25 @@
       <c r="C3">
         <v>29.699999999999999</v>
       </c>
-      <c r="D3">
-        <f>MAX(0,ROUND(B3/$H$2*224,1)-1)</f>
-        <v>33.399999999999999</v>
-      </c>
-      <c r="E3" s="2">
-        <f>MAX(0,ROUND(C3/$I$2*64,1)-1)</f>
+      <c r="D3" s="2">
+        <f>MAX(0,ROUND(B3/$K$2*224,1)-1)</f>
+        <v>11.700000000000001</v>
+      </c>
+      <c r="E3" s="3">
+        <f t="shared" si="0"/>
         <v>19.200000000000003</v>
       </c>
-      <c r="F3" s="3">
-        <f>B3/19</f>
+      <c r="F3" s="4">
+        <f t="shared" si="1"/>
         <v>1.1263157894736842</v>
       </c>
-      <c r="G3" s="4">
-        <f>C3/19</f>
+      <c r="G3" s="5">
+        <f t="shared" si="2"/>
         <v>1.5631578947368421</v>
       </c>
     </row>
     <row r="4" ht="14.25">
-      <c r="A4" s="5">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4">
@@ -731,25 +742,25 @@
       <c r="C4">
         <v>9.5999999999999996</v>
       </c>
-      <c r="D4">
-        <f>MAX(0,ROUND(B4/$H$2*224,1)-1)</f>
-        <v>67.700000000000003</v>
-      </c>
-      <c r="E4" s="2">
-        <f>MAX(0,ROUND(C4/$I$2*64,1)-1)</f>
+      <c r="D4" s="2">
+        <f>MAX(0,ROUND(B4/$K$2*224,1)-1)</f>
+        <v>24.300000000000001</v>
+      </c>
+      <c r="E4" s="3">
+        <f t="shared" si="0"/>
         <v>5.5</v>
       </c>
-      <c r="F4" s="3">
-        <f>B4/19</f>
+      <c r="F4" s="4">
+        <f t="shared" si="1"/>
         <v>2.2473684210526317</v>
       </c>
-      <c r="G4" s="4">
-        <f>C4/19</f>
+      <c r="G4" s="5">
+        <f t="shared" si="2"/>
         <v>0.50526315789473686</v>
       </c>
     </row>
     <row r="5" ht="14.25">
-      <c r="A5" s="5">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5">
@@ -758,25 +769,25 @@
       <c r="C5">
         <v>0</v>
       </c>
-      <c r="D5">
-        <f>MAX(0,ROUND(B5/$H$2*224,1)-1)</f>
-        <v>100.7</v>
-      </c>
-      <c r="E5" s="2">
-        <f>MAX(0,ROUND(C5/$I$2*64,1)-1)</f>
+      <c r="D5" s="2">
+        <f>MAX(0,ROUND(B5/$K$2*224,1)-1)</f>
+        <v>36.399999999999999</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F5" s="3">
-        <f>B5/19</f>
+      <c r="F5" s="4">
+        <f t="shared" si="1"/>
         <v>3.3263157894736843</v>
       </c>
-      <c r="G5" s="4">
-        <f>C5/19</f>
+      <c r="G5" s="5">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="6" ht="14.25">
-      <c r="A6" s="5">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6">
@@ -785,25 +796,25 @@
       <c r="C6">
         <v>16.100000000000001</v>
       </c>
-      <c r="D6">
-        <f>MAX(0,ROUND(B6/$H$2*224,1)-1)</f>
-        <v>132.09999999999999</v>
-      </c>
-      <c r="E6" s="2">
-        <f>MAX(0,ROUND(C6/$I$2*64,1)-1)</f>
+      <c r="D6" s="2">
+        <f>MAX(0,ROUND(B6/$K$2*224,1)-1)</f>
+        <v>48</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="0"/>
         <v>9.9000000000000004</v>
       </c>
-      <c r="F6" s="3">
-        <f>B6/19</f>
+      <c r="F6" s="4">
+        <f t="shared" si="1"/>
         <v>4.3526315789473689</v>
       </c>
-      <c r="G6" s="4">
-        <f>C6/19</f>
+      <c r="G6" s="5">
+        <f t="shared" si="2"/>
         <v>0.84736842105263166</v>
       </c>
     </row>
     <row r="7" ht="14.25">
-      <c r="A7" s="5">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7">
@@ -812,20 +823,20 @@
       <c r="C7">
         <v>18</v>
       </c>
-      <c r="D7">
-        <f>MAX(0,ROUND(B7/$H$2*224,1)-1)</f>
-        <v>166.5</v>
-      </c>
-      <c r="E7" s="2">
-        <f>MAX(0,ROUND(C7/$I$2*64,1)-1)</f>
+      <c r="D7" s="2">
+        <f>MAX(0,ROUND(B7/$K$2*224,1)-1)</f>
+        <v>60.600000000000001</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="0"/>
         <v>11.200000000000001</v>
       </c>
-      <c r="F7" s="3">
-        <f>B7/19</f>
+      <c r="F7" s="4">
+        <f t="shared" si="1"/>
         <v>5.4789473684210526</v>
       </c>
-      <c r="G7" s="4">
-        <f>C7/19</f>
+      <c r="G7" s="5">
+        <f t="shared" si="2"/>
         <v>0.94736842105263153</v>
       </c>
     </row>
@@ -840,20 +851,20 @@
       <c r="C8" s="6">
         <v>18</v>
       </c>
-      <c r="D8">
-        <f>MAX(0,ROUND(B8/$H$2*224,1)-1)</f>
-        <v>440.40000000000003</v>
-      </c>
-      <c r="E8" s="2">
-        <f>MAX(0,ROUND(C8/$I$2*64,1)-1)</f>
+      <c r="D8" s="2">
+        <f>MAX(0,ROUND(B8/$K$2*224,1)-1)</f>
+        <v>161.40000000000001</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="0"/>
         <v>11.200000000000001</v>
       </c>
-      <c r="F8" s="3">
-        <f>B8/19</f>
+      <c r="F8" s="4">
+        <f t="shared" si="1"/>
         <v>14.436842105263155</v>
       </c>
-      <c r="G8" s="4">
-        <f>C8/19</f>
+      <c r="G8" s="5">
+        <f t="shared" si="2"/>
         <v>0.94736842105263153</v>
       </c>
     </row>
@@ -868,20 +879,20 @@
       <c r="C9" s="6">
         <v>16.100000000000001</v>
       </c>
-      <c r="D9">
-        <f>MAX(0,ROUND(B9/$H$2*224,1)-1)</f>
-        <v>474.80000000000001</v>
-      </c>
-      <c r="E9" s="2">
-        <f>MAX(0,ROUND(C9/$I$2*64,1)-1)</f>
+      <c r="D9" s="2">
+        <f>MAX(0,ROUND(B9/$K$2*224,1)-1)</f>
+        <v>174</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="0"/>
         <v>9.9000000000000004</v>
       </c>
-      <c r="F9" s="3">
-        <f>B9/19</f>
+      <c r="F9" s="4">
+        <f t="shared" si="1"/>
         <v>15.563157894736841</v>
       </c>
-      <c r="G9" s="4">
-        <f>C9/19</f>
+      <c r="G9" s="5">
+        <f t="shared" si="2"/>
         <v>0.84736842105263166</v>
       </c>
     </row>
@@ -896,20 +907,20 @@
       <c r="C10" s="6">
         <v>0</v>
       </c>
-      <c r="D10">
-        <f>MAX(0,ROUND(B10/$H$2*224,1)-1)</f>
-        <v>506.20000000000005</v>
-      </c>
-      <c r="E10" s="2">
-        <f>MAX(0,ROUND(C10/$I$2*64,1)-1)</f>
+      <c r="D10" s="2">
+        <f>MAX(0,ROUND(B10/$K$2*224,1)-1)</f>
+        <v>185.60000000000002</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" ref="E10:E50" si="3">MAX(0,ROUND(C10/$I$2*64,1)-1)</f>
         <v>0</v>
       </c>
-      <c r="F10" s="3">
-        <f>B10/19</f>
+      <c r="F10" s="4">
+        <f t="shared" ref="F10:F51" si="4">B10/19</f>
         <v>16.589473684210525</v>
       </c>
-      <c r="G10" s="4">
-        <f>C10/19</f>
+      <c r="G10" s="5">
+        <f t="shared" ref="G10:G51" si="5">C10/19</f>
         <v>0</v>
       </c>
     </row>
@@ -924,20 +935,20 @@
       <c r="C11" s="6">
         <v>9.5999999999999996</v>
       </c>
-      <c r="D11">
-        <f>MAX(0,ROUND(B11/$H$2*224,1)-1)</f>
-        <v>539.20000000000005</v>
-      </c>
-      <c r="E11" s="2">
-        <f>MAX(0,ROUND(C11/$I$2*64,1)-1)</f>
+      <c r="D11" s="2">
+        <f>MAX(0,ROUND(B11/$K$2*224,1)-1)</f>
+        <v>197.70000000000002</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="3"/>
         <v>5.5</v>
       </c>
-      <c r="F11" s="3">
-        <f>B11/19</f>
+      <c r="F11" s="4">
+        <f t="shared" si="4"/>
         <v>17.668421052631579</v>
       </c>
-      <c r="G11" s="4">
-        <f>C11/19</f>
+      <c r="G11" s="5">
+        <f t="shared" si="5"/>
         <v>0.50526315789473686</v>
       </c>
     </row>
@@ -952,20 +963,20 @@
       <c r="C12" s="6">
         <v>29.699999999999999</v>
       </c>
-      <c r="D12">
-        <f>MAX(0,ROUND(B12/$H$2*224,1)-1)</f>
-        <v>573.5</v>
-      </c>
-      <c r="E12" s="2">
-        <f>MAX(0,ROUND(C12/$I$2*64,1)-1)</f>
+      <c r="D12" s="2">
+        <f>MAX(0,ROUND(B12/$K$2*224,1)-1)</f>
+        <v>210.30000000000001</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="3"/>
         <v>19.200000000000003</v>
       </c>
-      <c r="F12" s="3">
-        <f>B12/19</f>
+      <c r="F12" s="4">
+        <f t="shared" si="4"/>
         <v>18.789473684210527</v>
       </c>
-      <c r="G12" s="4">
-        <f>C12/19</f>
+      <c r="G12" s="5">
+        <f t="shared" si="5"/>
         <v>1.5631578947368421</v>
       </c>
     </row>
@@ -980,25 +991,25 @@
       <c r="C13" s="6">
         <v>30.899999999999999</v>
       </c>
-      <c r="D13">
-        <f>MAX(0,ROUND(B13/$H$2*224,1)-1)</f>
-        <v>607.89999999999998</v>
-      </c>
-      <c r="E13" s="2">
-        <f>MAX(0,ROUND(C13/$I$2*64,1)-1)</f>
+      <c r="D13" s="2">
+        <f>MAX(0,ROUND(B13/$K$2*224,1)-1)</f>
+        <v>223</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="F13" s="3">
-        <f>B13/19</f>
+      <c r="F13" s="4">
+        <f t="shared" si="4"/>
         <v>19.91578947368421</v>
       </c>
-      <c r="G13" s="4">
-        <f>C13/19</f>
+      <c r="G13" s="5">
+        <f t="shared" si="5"/>
         <v>1.6263157894736842</v>
       </c>
     </row>
     <row r="14" ht="14.25">
-      <c r="A14" s="5">
+      <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14">
@@ -1007,25 +1018,25 @@
       <c r="C14">
         <v>49.799999999999997</v>
       </c>
-      <c r="D14">
-        <f>MAX(0,ROUND(B14/$H$2*224,1)-1)</f>
-        <v>1.6000000000000001</v>
-      </c>
-      <c r="E14" s="2">
-        <f>MAX(0,ROUND(C14/$I$2*64,1)-1)</f>
+      <c r="D14" s="2">
+        <f>MAX(0,ROUND(B14/$K$2*224,1)-1)</f>
+        <v>0</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="3"/>
         <v>32.800000000000004</v>
       </c>
-      <c r="F14" s="3">
-        <f>B14/19</f>
+      <c r="F14" s="4">
+        <f t="shared" si="4"/>
         <v>0.084210526315789472</v>
       </c>
-      <c r="G14" s="4">
-        <f>C14/19</f>
+      <c r="G14" s="5">
+        <f t="shared" si="5"/>
         <v>2.6210526315789471</v>
       </c>
     </row>
     <row r="15" ht="14.25">
-      <c r="A15" s="5">
+      <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15">
@@ -1034,25 +1045,25 @@
       <c r="C15">
         <v>48.700000000000003</v>
       </c>
-      <c r="D15">
-        <f>MAX(0,ROUND(B15/$H$2*224,1)-1)</f>
-        <v>34.600000000000001</v>
-      </c>
-      <c r="E15" s="2">
-        <f>MAX(0,ROUND(C15/$I$2*64,1)-1)</f>
+      <c r="D15" s="2">
+        <f>MAX(0,ROUND(B15/$K$2*224,1)-1)</f>
+        <v>12.100000000000001</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="3"/>
         <v>32.100000000000001</v>
       </c>
-      <c r="F15" s="3">
-        <f>B15/19</f>
+      <c r="F15" s="4">
+        <f t="shared" si="4"/>
         <v>1.1631578947368422</v>
       </c>
-      <c r="G15" s="4">
-        <f>C15/19</f>
+      <c r="G15" s="5">
+        <f t="shared" si="5"/>
         <v>2.5631578947368423</v>
       </c>
     </row>
     <row r="16" ht="14.25">
-      <c r="A16" s="5">
+      <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16">
@@ -1061,25 +1072,25 @@
       <c r="C16">
         <v>28.600000000000001</v>
       </c>
-      <c r="D16">
-        <f>MAX(0,ROUND(B16/$H$2*224,1)-1)</f>
-        <v>67.100000000000009</v>
-      </c>
-      <c r="E16" s="2">
-        <f>MAX(0,ROUND(C16/$I$2*64,1)-1)</f>
+      <c r="D16" s="2">
+        <f>MAX(0,ROUND(B16/$K$2*224,1)-1)</f>
+        <v>24</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="3"/>
         <v>18.400000000000002</v>
       </c>
-      <c r="F16" s="3">
-        <f>B16/19</f>
+      <c r="F16" s="4">
+        <f t="shared" si="4"/>
         <v>2.2263157894736842</v>
       </c>
-      <c r="G16" s="4">
-        <f>C16/19</f>
+      <c r="G16" s="5">
+        <f t="shared" si="5"/>
         <v>1.5052631578947369</v>
       </c>
     </row>
     <row r="17" ht="14.25">
-      <c r="A17" s="5">
+      <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17">
@@ -1088,25 +1099,25 @@
       <c r="C17">
         <v>19</v>
       </c>
-      <c r="D17">
-        <f>MAX(0,ROUND(B17/$H$2*224,1)-1)</f>
-        <v>99.100000000000009</v>
-      </c>
-      <c r="E17" s="2">
-        <f>MAX(0,ROUND(C17/$I$2*64,1)-1)</f>
+      <c r="D17" s="2">
+        <f>MAX(0,ROUND(B17/$K$2*224,1)-1)</f>
+        <v>35.800000000000004</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="3"/>
         <v>11.9</v>
       </c>
-      <c r="F17" s="3">
-        <f>B17/19</f>
+      <c r="F17" s="4">
+        <f t="shared" si="4"/>
         <v>3.2736842105263158</v>
       </c>
-      <c r="G17" s="4">
-        <f>C17/19</f>
+      <c r="G17" s="5">
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="18" ht="14.25">
-      <c r="A18" s="5">
+      <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18">
@@ -1115,25 +1126,25 @@
       <c r="C18">
         <v>35</v>
       </c>
-      <c r="D18">
-        <f>MAX(0,ROUND(B18/$H$2*224,1)-1)</f>
-        <v>129.30000000000001</v>
-      </c>
-      <c r="E18" s="2">
-        <f>MAX(0,ROUND(C18/$I$2*64,1)-1)</f>
+      <c r="D18" s="2">
+        <f>MAX(0,ROUND(B18/$K$2*224,1)-1)</f>
+        <v>46.900000000000006</v>
+      </c>
+      <c r="E18" s="3">
+        <f t="shared" si="3"/>
         <v>22.800000000000001</v>
       </c>
-      <c r="F18" s="3">
-        <f>B18/19</f>
+      <c r="F18" s="4">
+        <f t="shared" si="4"/>
         <v>4.2631578947368425</v>
       </c>
-      <c r="G18" s="4">
-        <f>C18/19</f>
+      <c r="G18" s="5">
+        <f t="shared" si="5"/>
         <v>1.8421052631578947</v>
       </c>
     </row>
     <row r="19" ht="14.25">
-      <c r="A19" s="5">
+      <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19">
@@ -1142,20 +1153,20 @@
       <c r="C19">
         <v>36.799999999999997</v>
       </c>
-      <c r="D19">
-        <f>MAX(0,ROUND(B19/$H$2*224,1)-1)</f>
-        <v>162.30000000000001</v>
-      </c>
-      <c r="E19" s="2">
-        <f>MAX(0,ROUND(C19/$I$2*64,1)-1)</f>
+      <c r="D19" s="2">
+        <f>MAX(0,ROUND(B19/$K$2*224,1)-1)</f>
+        <v>59.100000000000001</v>
+      </c>
+      <c r="E19" s="3">
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
-      <c r="F19" s="3">
-        <f>B19/19</f>
+      <c r="F19" s="4">
+        <f t="shared" si="4"/>
         <v>5.3421052631578947</v>
       </c>
-      <c r="G19" s="4">
-        <f>C19/19</f>
+      <c r="G19" s="5">
+        <f t="shared" si="5"/>
         <v>1.9368421052631577</v>
       </c>
     </row>
@@ -1170,20 +1181,20 @@
       <c r="C20" s="6">
         <v>36.799999999999997</v>
       </c>
-      <c r="D20">
-        <f>MAX(0,ROUND(B20/$H$2*224,1)-1)</f>
-        <v>444.60000000000002</v>
-      </c>
-      <c r="E20" s="2">
-        <f>MAX(0,ROUND(C20/$I$2*64,1)-1)</f>
+      <c r="D20" s="2">
+        <f>MAX(0,ROUND(B20/$K$2*224,1)-1)</f>
+        <v>162.90000000000001</v>
+      </c>
+      <c r="E20" s="3">
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
-      <c r="F20" s="3">
-        <f>B20/19</f>
+      <c r="F20" s="4">
+        <f t="shared" si="4"/>
         <v>14.573684210526315</v>
       </c>
-      <c r="G20" s="4">
-        <f>C20/19</f>
+      <c r="G20" s="5">
+        <f t="shared" si="5"/>
         <v>1.9368421052631577</v>
       </c>
     </row>
@@ -1198,20 +1209,20 @@
       <c r="C21" s="6">
         <v>35</v>
       </c>
-      <c r="D21">
-        <f>MAX(0,ROUND(B21/$H$2*224,1)-1)</f>
-        <v>477.60000000000002</v>
-      </c>
-      <c r="E21" s="2">
-        <f>MAX(0,ROUND(C21/$I$2*64,1)-1)</f>
+      <c r="D21" s="2">
+        <f>MAX(0,ROUND(B21/$K$2*224,1)-1)</f>
+        <v>175.10000000000002</v>
+      </c>
+      <c r="E21" s="3">
+        <f t="shared" si="3"/>
         <v>22.800000000000001</v>
       </c>
-      <c r="F21" s="3">
-        <f>B21/19</f>
+      <c r="F21" s="4">
+        <f t="shared" si="4"/>
         <v>15.652631578947368</v>
       </c>
-      <c r="G21" s="4">
-        <f>C21/19</f>
+      <c r="G21" s="5">
+        <f t="shared" si="5"/>
         <v>1.8421052631578947</v>
       </c>
     </row>
@@ -1226,20 +1237,20 @@
       <c r="C22" s="6">
         <v>19</v>
       </c>
-      <c r="D22">
-        <f>MAX(0,ROUND(B22/$H$2*224,1)-1)</f>
-        <v>507.80000000000001</v>
-      </c>
-      <c r="E22" s="2">
-        <f>MAX(0,ROUND(C22/$I$2*64,1)-1)</f>
+      <c r="D22" s="2">
+        <f>MAX(0,ROUND(B22/$K$2*224,1)-1)</f>
+        <v>186.20000000000002</v>
+      </c>
+      <c r="E22" s="3">
+        <f t="shared" si="3"/>
         <v>11.9</v>
       </c>
-      <c r="F22" s="3">
-        <f>B22/19</f>
+      <c r="F22" s="4">
+        <f t="shared" si="4"/>
         <v>16.642105263157895</v>
       </c>
-      <c r="G22" s="4">
-        <f>C22/19</f>
+      <c r="G22" s="5">
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -1254,20 +1265,20 @@
       <c r="C23" s="6">
         <v>28.600000000000001</v>
       </c>
-      <c r="D23">
-        <f>MAX(0,ROUND(B23/$H$2*224,1)-1)</f>
-        <v>539.89999999999998</v>
-      </c>
-      <c r="E23" s="2">
-        <f>MAX(0,ROUND(C23/$I$2*64,1)-1)</f>
+      <c r="D23" s="2">
+        <f>MAX(0,ROUND(B23/$K$2*224,1)-1)</f>
+        <v>198</v>
+      </c>
+      <c r="E23" s="3">
+        <f t="shared" si="3"/>
         <v>18.400000000000002</v>
       </c>
-      <c r="F23" s="3">
-        <f>B23/19</f>
+      <c r="F23" s="4">
+        <f t="shared" si="4"/>
         <v>17.689473684210526</v>
       </c>
-      <c r="G23" s="4">
-        <f>C23/19</f>
+      <c r="G23" s="5">
+        <f t="shared" si="5"/>
         <v>1.5052631578947369</v>
       </c>
     </row>
@@ -1282,20 +1293,20 @@
       <c r="C24" s="6">
         <v>48.700000000000003</v>
       </c>
-      <c r="D24">
-        <f>MAX(0,ROUND(B24/$H$2*224,1)-1)</f>
-        <v>572.39999999999998</v>
-      </c>
-      <c r="E24" s="2">
-        <f>MAX(0,ROUND(C24/$I$2*64,1)-1)</f>
+      <c r="D24" s="2">
+        <f>MAX(0,ROUND(B24/$K$2*224,1)-1)</f>
+        <v>209.90000000000001</v>
+      </c>
+      <c r="E24" s="3">
+        <f t="shared" si="3"/>
         <v>32.100000000000001</v>
       </c>
-      <c r="F24" s="3">
-        <f>B24/19</f>
+      <c r="F24" s="4">
+        <f t="shared" si="4"/>
         <v>18.752631578947366</v>
       </c>
-      <c r="G24" s="4">
-        <f>C24/19</f>
+      <c r="G24" s="5">
+        <f t="shared" si="5"/>
         <v>2.5631578947368423</v>
       </c>
     </row>
@@ -1310,25 +1321,25 @@
       <c r="C25" s="6">
         <v>49.799999999999997</v>
       </c>
-      <c r="D25">
-        <f>MAX(0,ROUND(B25/$H$2*224,1)-1)</f>
-        <v>605.30000000000007</v>
-      </c>
-      <c r="E25" s="2">
-        <f>MAX(0,ROUND(C25/$I$2*64,1)-1)</f>
+      <c r="D25" s="2">
+        <f>MAX(0,ROUND(B25/$K$2*224,1)-1)</f>
+        <v>222.10000000000002</v>
+      </c>
+      <c r="E25" s="3">
+        <f t="shared" si="3"/>
         <v>32.800000000000004</v>
       </c>
-      <c r="F25" s="3">
-        <f>B25/19</f>
+      <c r="F25" s="4">
+        <f t="shared" si="4"/>
         <v>19.831578947368417</v>
       </c>
-      <c r="G25" s="4">
-        <f>C25/19</f>
+      <c r="G25" s="5">
+        <f t="shared" si="5"/>
         <v>2.6210526315789471</v>
       </c>
     </row>
     <row r="26" ht="14.25">
-      <c r="A26" s="5">
+      <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26">
@@ -1337,25 +1348,25 @@
       <c r="C26">
         <v>68.700000000000003</v>
       </c>
-      <c r="D26">
-        <f>MAX(0,ROUND(B26/$H$2*224,1)-1)</f>
-        <v>4.3000000000000007</v>
-      </c>
-      <c r="E26" s="2">
-        <f>MAX(0,ROUND(C26/$I$2*64,1)-1)</f>
+      <c r="D26" s="2">
+        <f>MAX(0,ROUND(B26/$K$2*224,1)-1)</f>
+        <v>1</v>
+      </c>
+      <c r="E26" s="3">
+        <f t="shared" si="3"/>
         <v>45.700000000000003</v>
       </c>
-      <c r="F26" s="3">
-        <f>B26/19</f>
+      <c r="F26" s="4">
+        <f t="shared" si="4"/>
         <v>0.17368421052631577</v>
       </c>
-      <c r="G26" s="4">
-        <f>C26/19</f>
+      <c r="G26" s="5">
+        <f t="shared" si="5"/>
         <v>3.6157894736842109</v>
       </c>
     </row>
     <row r="27" ht="14.25">
-      <c r="A27" s="5">
+      <c r="A27" s="1">
         <v>25</v>
       </c>
       <c r="B27">
@@ -1364,25 +1375,25 @@
       <c r="C27">
         <v>67.599999999999994</v>
       </c>
-      <c r="D27">
-        <f>MAX(0,ROUND(B27/$H$2*224,1)-1)</f>
-        <v>35.600000000000001</v>
-      </c>
-      <c r="E27" s="2">
-        <f>MAX(0,ROUND(C27/$I$2*64,1)-1)</f>
+      <c r="D27" s="2">
+        <f>MAX(0,ROUND(B27/$K$2*224,1)-1)</f>
+        <v>12.5</v>
+      </c>
+      <c r="E27" s="3">
+        <f t="shared" si="3"/>
         <v>44.900000000000006</v>
       </c>
-      <c r="F27" s="3">
-        <f>B27/19</f>
+      <c r="F27" s="4">
+        <f t="shared" si="4"/>
         <v>1.1973684210526316</v>
       </c>
-      <c r="G27" s="4">
-        <f>C27/19</f>
+      <c r="G27" s="5">
+        <f t="shared" si="5"/>
         <v>3.5578947368421048</v>
       </c>
     </row>
     <row r="28" ht="14.25">
-      <c r="A28" s="5">
+      <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="B28">
@@ -1391,25 +1402,25 @@
       <c r="C28">
         <v>47.600000000000001</v>
       </c>
-      <c r="D28">
-        <f>MAX(0,ROUND(B28/$H$2*224,1)-1)</f>
-        <v>66.600000000000009</v>
-      </c>
-      <c r="E28" s="2">
-        <f>MAX(0,ROUND(C28/$I$2*64,1)-1)</f>
+      <c r="D28" s="2">
+        <f>MAX(0,ROUND(B28/$K$2*224,1)-1)</f>
+        <v>23.900000000000002</v>
+      </c>
+      <c r="E28" s="3">
+        <f t="shared" si="3"/>
         <v>31.300000000000004</v>
       </c>
-      <c r="F28" s="3">
-        <f>B28/19</f>
+      <c r="F28" s="4">
+        <f t="shared" si="4"/>
         <v>2.2105263157894739</v>
       </c>
-      <c r="G28" s="4">
-        <f>C28/19</f>
+      <c r="G28" s="5">
+        <f t="shared" si="5"/>
         <v>2.5052631578947371</v>
       </c>
     </row>
     <row r="29" ht="14.25">
-      <c r="A29" s="5">
+      <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="B29">
@@ -1418,25 +1429,25 @@
       <c r="C29">
         <v>38</v>
       </c>
-      <c r="D29">
-        <f>MAX(0,ROUND(B29/$H$2*224,1)-1)</f>
-        <v>97.5</v>
-      </c>
-      <c r="E29" s="2">
-        <f>MAX(0,ROUND(C29/$I$2*64,1)-1)</f>
+      <c r="D29" s="2">
+        <f>MAX(0,ROUND(B29/$K$2*224,1)-1)</f>
+        <v>35.200000000000003</v>
+      </c>
+      <c r="E29" s="3">
+        <f t="shared" si="3"/>
         <v>24.800000000000001</v>
       </c>
-      <c r="F29" s="3">
-        <f>B29/19</f>
+      <c r="F29" s="4">
+        <f t="shared" si="4"/>
         <v>3.2210526315789476</v>
       </c>
-      <c r="G29" s="4">
-        <f>C29/19</f>
+      <c r="G29" s="5">
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
     <row r="30" ht="14.25">
-      <c r="A30" s="5">
+      <c r="A30" s="1">
         <v>28</v>
       </c>
       <c r="B30">
@@ -1445,25 +1456,25 @@
       <c r="C30">
         <v>53.899999999999999</v>
       </c>
-      <c r="D30">
-        <f>MAX(0,ROUND(B30/$H$2*224,1)-1)</f>
-        <v>126.80000000000001</v>
-      </c>
-      <c r="E30" s="2">
-        <f>MAX(0,ROUND(C30/$I$2*64,1)-1)</f>
+      <c r="D30" s="2">
+        <f>MAX(0,ROUND(B30/$K$2*224,1)-1)</f>
+        <v>46</v>
+      </c>
+      <c r="E30" s="3">
+        <f t="shared" si="3"/>
         <v>35.600000000000001</v>
       </c>
-      <c r="F30" s="3">
-        <f>B30/19</f>
+      <c r="F30" s="4">
+        <f t="shared" si="4"/>
         <v>4.1789473684210527</v>
       </c>
-      <c r="G30" s="4">
-        <f>C30/19</f>
+      <c r="G30" s="5">
+        <f t="shared" si="5"/>
         <v>2.8368421052631576</v>
       </c>
     </row>
     <row r="31" ht="14.25">
-      <c r="A31" s="5">
+      <c r="A31" s="1">
         <v>29</v>
       </c>
       <c r="B31">
@@ -1472,20 +1483,20 @@
       <c r="C31">
         <v>55.600000000000001</v>
       </c>
-      <c r="D31">
-        <f>MAX(0,ROUND(B31/$H$2*224,1)-1)</f>
-        <v>158.10000000000002</v>
-      </c>
-      <c r="E31" s="2">
-        <f>MAX(0,ROUND(C31/$I$2*64,1)-1)</f>
+      <c r="D31" s="2">
+        <f>MAX(0,ROUND(B31/$K$2*224,1)-1)</f>
+        <v>57.5</v>
+      </c>
+      <c r="E31" s="3">
+        <f t="shared" si="3"/>
         <v>36.800000000000004</v>
       </c>
-      <c r="F31" s="3">
-        <f>B31/19</f>
+      <c r="F31" s="4">
+        <f t="shared" si="4"/>
         <v>5.2052631578947368</v>
       </c>
-      <c r="G31" s="4">
-        <f>C31/19</f>
+      <c r="G31" s="5">
+        <f t="shared" si="5"/>
         <v>2.9263157894736844</v>
       </c>
     </row>
@@ -1500,20 +1511,20 @@
       <c r="C32" s="6">
         <v>55.600000000000001</v>
       </c>
-      <c r="D32">
-        <f>MAX(0,ROUND(B32/$H$2*224,1)-1)</f>
-        <v>448.80000000000001</v>
-      </c>
-      <c r="E32" s="2">
-        <f>MAX(0,ROUND(C32/$I$2*64,1)-1)</f>
+      <c r="D32" s="2">
+        <f>MAX(0,ROUND(B32/$K$2*224,1)-1)</f>
+        <v>164.5</v>
+      </c>
+      <c r="E32" s="3">
+        <f t="shared" si="3"/>
         <v>36.800000000000004</v>
       </c>
-      <c r="F32" s="3">
-        <f>B32/19</f>
+      <c r="F32" s="4">
+        <f t="shared" si="4"/>
         <v>14.710526315789474</v>
       </c>
-      <c r="G32" s="4">
-        <f>C32/19</f>
+      <c r="G32" s="5">
+        <f t="shared" si="5"/>
         <v>2.9263157894736844</v>
       </c>
     </row>
@@ -1528,20 +1539,20 @@
       <c r="C33" s="6">
         <v>53.899999999999999</v>
       </c>
-      <c r="D33">
-        <f>MAX(0,ROUND(B33/$H$2*224,1)-1)</f>
-        <v>480.10000000000002</v>
-      </c>
-      <c r="E33" s="2">
-        <f>MAX(0,ROUND(C33/$I$2*64,1)-1)</f>
+      <c r="D33" s="2">
+        <f>MAX(0,ROUND(B33/$K$2*224,1)-1)</f>
+        <v>176</v>
+      </c>
+      <c r="E33" s="3">
+        <f t="shared" si="3"/>
         <v>35.600000000000001</v>
       </c>
-      <c r="F33" s="3">
-        <f>B33/19</f>
+      <c r="F33" s="4">
+        <f t="shared" si="4"/>
         <v>15.736842105263158</v>
       </c>
-      <c r="G33" s="4">
-        <f>C33/19</f>
+      <c r="G33" s="5">
+        <f t="shared" si="5"/>
         <v>2.8368421052631576</v>
       </c>
     </row>
@@ -1556,20 +1567,20 @@
       <c r="C34" s="6">
         <v>38</v>
       </c>
-      <c r="D34">
-        <f>MAX(0,ROUND(B34/$H$2*224,1)-1)</f>
-        <v>509.40000000000003</v>
-      </c>
-      <c r="E34" s="2">
-        <f>MAX(0,ROUND(C34/$I$2*64,1)-1)</f>
+      <c r="D34" s="2">
+        <f>MAX(0,ROUND(B34/$K$2*224,1)-1)</f>
+        <v>186.80000000000001</v>
+      </c>
+      <c r="E34" s="3">
+        <f t="shared" si="3"/>
         <v>24.800000000000001</v>
       </c>
-      <c r="F34" s="3">
-        <f>B34/19</f>
+      <c r="F34" s="4">
+        <f t="shared" si="4"/>
         <v>16.694736842105261</v>
       </c>
-      <c r="G34" s="4">
-        <f>C34/19</f>
+      <c r="G34" s="5">
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
@@ -1584,20 +1595,20 @@
       <c r="C35" s="6">
         <v>47.600000000000001</v>
       </c>
-      <c r="D35">
-        <f>MAX(0,ROUND(B35/$H$2*224,1)-1)</f>
-        <v>540.30000000000007</v>
-      </c>
-      <c r="E35" s="2">
-        <f>MAX(0,ROUND(C35/$I$2*64,1)-1)</f>
+      <c r="D35" s="2">
+        <f>MAX(0,ROUND(B35/$K$2*224,1)-1)</f>
+        <v>198.10000000000002</v>
+      </c>
+      <c r="E35" s="3">
+        <f t="shared" si="3"/>
         <v>31.300000000000004</v>
       </c>
-      <c r="F35" s="3">
-        <f>B35/19</f>
+      <c r="F35" s="4">
+        <f t="shared" si="4"/>
         <v>17.705263157894734</v>
       </c>
-      <c r="G35" s="4">
-        <f>C35/19</f>
+      <c r="G35" s="5">
+        <f t="shared" si="5"/>
         <v>2.5052631578947371</v>
       </c>
     </row>
@@ -1612,20 +1623,20 @@
       <c r="C36" s="6">
         <v>67.599999999999994</v>
       </c>
-      <c r="D36">
-        <f>MAX(0,ROUND(B36/$H$2*224,1)-1)</f>
-        <v>571.30000000000007</v>
-      </c>
-      <c r="E36" s="2">
-        <f>MAX(0,ROUND(C36/$I$2*64,1)-1)</f>
+      <c r="D36" s="2">
+        <f>MAX(0,ROUND(B36/$K$2*224,1)-1)</f>
+        <v>209.5</v>
+      </c>
+      <c r="E36" s="3">
+        <f t="shared" si="3"/>
         <v>44.900000000000006</v>
       </c>
-      <c r="F36" s="3">
-        <f>B36/19</f>
+      <c r="F36" s="4">
+        <f t="shared" si="4"/>
         <v>18.718421052631577</v>
       </c>
-      <c r="G36" s="4">
-        <f>C36/19</f>
+      <c r="G36" s="5">
+        <f t="shared" si="5"/>
         <v>3.5578947368421048</v>
       </c>
     </row>
@@ -1640,25 +1651,25 @@
       <c r="C37" s="6">
         <v>68.700000000000003</v>
       </c>
-      <c r="D37">
-        <f>MAX(0,ROUND(B37/$H$2*224,1)-1)</f>
-        <v>602.60000000000002</v>
-      </c>
-      <c r="E37" s="2">
-        <f>MAX(0,ROUND(C37/$I$2*64,1)-1)</f>
+      <c r="D37" s="2">
+        <f>MAX(0,ROUND(B37/$K$2*224,1)-1)</f>
+        <v>221</v>
+      </c>
+      <c r="E37" s="3">
+        <f t="shared" si="3"/>
         <v>45.700000000000003</v>
       </c>
-      <c r="F37" s="3">
-        <f>B37/19</f>
+      <c r="F37" s="4">
+        <f t="shared" si="4"/>
         <v>19.742105263157892</v>
       </c>
-      <c r="G37" s="4">
-        <f>C37/19</f>
+      <c r="G37" s="5">
+        <f t="shared" si="5"/>
         <v>3.6157894736842109</v>
       </c>
     </row>
     <row r="38" ht="14.25">
-      <c r="A38" s="5">
+      <c r="A38" s="1">
         <v>36</v>
       </c>
       <c r="B38">
@@ -1667,25 +1678,25 @@
       <c r="C38">
         <v>73.900000000000006</v>
       </c>
-      <c r="D38">
-        <f>MAX(0,ROUND(B38/$H$2*224,1)-1)</f>
-        <v>95.100000000000009</v>
-      </c>
-      <c r="E38" s="2">
-        <f>MAX(0,ROUND(C38/$I$2*64,1)-1)</f>
+      <c r="D38" s="2">
+        <f>MAX(0,ROUND(B38/$K$2*224,1)-1)</f>
+        <v>34.300000000000004</v>
+      </c>
+      <c r="E38" s="3">
+        <f t="shared" si="3"/>
         <v>49.200000000000003</v>
       </c>
-      <c r="F38" s="3">
-        <f>B38/19</f>
+      <c r="F38" s="4">
+        <f t="shared" si="4"/>
         <v>3.142105263157895</v>
       </c>
-      <c r="G38" s="4">
-        <f>C38/19</f>
+      <c r="G38" s="5">
+        <f t="shared" si="5"/>
         <v>3.8894736842105266</v>
       </c>
     </row>
     <row r="39" ht="14.25">
-      <c r="A39" s="5">
+      <c r="A39" s="1">
         <v>37</v>
       </c>
       <c r="B39">
@@ -1694,20 +1705,20 @@
       <c r="C39">
         <v>75.200000000000003</v>
       </c>
-      <c r="D39">
-        <f>MAX(0,ROUND(B39/$H$2*224,1)-1)</f>
-        <v>125.5</v>
-      </c>
-      <c r="E39" s="2">
-        <f>MAX(0,ROUND(C39/$I$2*64,1)-1)</f>
+      <c r="D39" s="2">
+        <f>MAX(0,ROUND(B39/$K$2*224,1)-1)</f>
+        <v>45.5</v>
+      </c>
+      <c r="E39" s="3">
+        <f t="shared" si="3"/>
         <v>50.100000000000001</v>
       </c>
-      <c r="F39" s="3">
-        <f>B39/19</f>
+      <c r="F39" s="4">
+        <f t="shared" si="4"/>
         <v>4.1368421052631579</v>
       </c>
-      <c r="G39" s="4">
-        <f>C39/19</f>
+      <c r="G39" s="5">
+        <f t="shared" si="5"/>
         <v>3.9578947368421056</v>
       </c>
     </row>
@@ -1722,20 +1733,20 @@
       <c r="C40" s="6">
         <v>75.200000000000003</v>
       </c>
-      <c r="D40">
-        <f>MAX(0,ROUND(B40/$H$2*224,1)-1)</f>
-        <v>481.40000000000003</v>
-      </c>
-      <c r="E40" s="2">
-        <f>MAX(0,ROUND(C40/$I$2*64,1)-1)</f>
+      <c r="D40" s="2">
+        <f>MAX(0,ROUND(B40/$K$2*224,1)-1)</f>
+        <v>176.5</v>
+      </c>
+      <c r="E40" s="3">
+        <f t="shared" si="3"/>
         <v>50.100000000000001</v>
       </c>
-      <c r="F40" s="3">
-        <f>B40/19</f>
+      <c r="F40" s="4">
+        <f t="shared" si="4"/>
         <v>15.778947368421051</v>
       </c>
-      <c r="G40" s="4">
-        <f>C40/19</f>
+      <c r="G40" s="5">
+        <f t="shared" si="5"/>
         <v>3.9578947368421056</v>
       </c>
     </row>
@@ -1750,25 +1761,25 @@
       <c r="C41" s="6">
         <v>73.900000000000006</v>
       </c>
-      <c r="D41">
-        <f>MAX(0,ROUND(B41/$H$2*224,1)-1)</f>
-        <v>511.89999999999998</v>
-      </c>
-      <c r="E41" s="2">
-        <f>MAX(0,ROUND(C41/$I$2*64,1)-1)</f>
+      <c r="D41" s="2">
+        <f>MAX(0,ROUND(B41/$K$2*224,1)-1)</f>
+        <v>187.70000000000002</v>
+      </c>
+      <c r="E41" s="3">
+        <f t="shared" si="3"/>
         <v>49.200000000000003</v>
       </c>
-      <c r="F41" s="3">
-        <f>B41/19</f>
+      <c r="F41" s="4">
+        <f t="shared" si="4"/>
         <v>16.773684210526316</v>
       </c>
-      <c r="G41" s="4">
-        <f>C41/19</f>
+      <c r="G41" s="5">
+        <f t="shared" si="5"/>
         <v>3.8894736842105266</v>
       </c>
     </row>
     <row r="42" ht="14.25">
-      <c r="A42" s="5">
+      <c r="A42" s="1">
         <v>40</v>
       </c>
       <c r="B42">
@@ -1777,25 +1788,25 @@
       <c r="C42">
         <v>92.900000000000006</v>
       </c>
-      <c r="D42">
-        <f>MAX(0,ROUND(B42/$H$2*224,1)-1)</f>
-        <v>92.800000000000011</v>
-      </c>
-      <c r="E42" s="2">
-        <f>MAX(0,ROUND(C42/$I$2*64,1)-1)</f>
+      <c r="D42" s="2">
+        <f>MAX(0,ROUND(B42/$K$2*224,1)-1)</f>
+        <v>33.5</v>
+      </c>
+      <c r="E42" s="3">
+        <f t="shared" si="3"/>
         <v>62.100000000000001</v>
       </c>
-      <c r="F42" s="3">
-        <f>B42/19</f>
+      <c r="F42" s="4">
+        <f t="shared" si="4"/>
         <v>3.0684210526315789</v>
       </c>
-      <c r="G42" s="4">
-        <f>C42/19</f>
+      <c r="G42" s="5">
+        <f t="shared" si="5"/>
         <v>4.8894736842105262</v>
       </c>
     </row>
     <row r="43" ht="14.25">
-      <c r="A43" s="5">
+      <c r="A43" s="1">
         <v>41</v>
       </c>
       <c r="B43">
@@ -1804,25 +1815,25 @@
       <c r="C43">
         <v>94.200000000000003</v>
       </c>
-      <c r="D43">
-        <f>MAX(0,ROUND(B43/$H$2*224,1)-1)</f>
-        <v>123.40000000000001</v>
-      </c>
-      <c r="E43" s="2">
-        <f>MAX(0,ROUND(C43/$I$2*64,1)-1)</f>
+      <c r="D43" s="2">
+        <f>MAX(0,ROUND(B43/$K$2*224,1)-1)</f>
+        <v>44.800000000000004</v>
+      </c>
+      <c r="E43" s="3">
+        <f t="shared" si="3"/>
         <v>63</v>
       </c>
-      <c r="F43" s="3">
-        <f>B43/19</f>
+      <c r="F43" s="4">
+        <f t="shared" si="4"/>
         <v>4.0684210526315789</v>
       </c>
-      <c r="G43" s="4">
-        <f>C43/19</f>
+      <c r="G43" s="5">
+        <f t="shared" si="5"/>
         <v>4.9578947368421051</v>
       </c>
     </row>
     <row r="44" ht="14.25">
-      <c r="A44" s="5">
+      <c r="A44" s="1">
         <v>42</v>
       </c>
       <c r="B44">
@@ -1831,25 +1842,25 @@
       <c r="C44">
         <v>86</v>
       </c>
-      <c r="D44">
-        <f>MAX(0,ROUND(B44/$H$2*224,1)-1)</f>
-        <v>154.90000000000001</v>
-      </c>
-      <c r="E44" s="2">
-        <f>MAX(0,ROUND(C44/$I$2*64,1)-1)</f>
+      <c r="D44" s="2">
+        <f>MAX(0,ROUND(B44/$K$2*224,1)-1)</f>
+        <v>56.400000000000006</v>
+      </c>
+      <c r="E44" s="3">
+        <f t="shared" si="3"/>
         <v>57.400000000000006</v>
       </c>
-      <c r="F44" s="3">
-        <f>B44/19</f>
+      <c r="F44" s="4">
+        <f t="shared" si="4"/>
         <v>5.1000000000000005</v>
       </c>
-      <c r="G44" s="4">
-        <f>C44/19</f>
+      <c r="G44" s="5">
+        <f t="shared" si="5"/>
         <v>4.5263157894736841</v>
       </c>
     </row>
     <row r="45" ht="14.25">
-      <c r="A45" s="5">
+      <c r="A45" s="1">
         <v>43</v>
       </c>
       <c r="B45">
@@ -1858,25 +1869,25 @@
       <c r="C45">
         <v>88.599999999999994</v>
       </c>
-      <c r="D45">
-        <f>MAX(0,ROUND(B45/$H$2*224,1)-1)</f>
-        <v>187.40000000000001</v>
-      </c>
-      <c r="E45" s="2">
-        <f>MAX(0,ROUND(C45/$I$2*64,1)-1)</f>
+      <c r="D45" s="2">
+        <f>MAX(0,ROUND(B45/$K$2*224,1)-1)</f>
+        <v>68.299999999999997</v>
+      </c>
+      <c r="E45" s="3">
+        <f t="shared" si="3"/>
         <v>59.200000000000003</v>
       </c>
-      <c r="F45" s="3">
-        <f>B45/19</f>
+      <c r="F45" s="4">
+        <f t="shared" si="4"/>
         <v>6.1631578947368419</v>
       </c>
-      <c r="G45" s="4">
-        <f>C45/19</f>
+      <c r="G45" s="5">
+        <f t="shared" si="5"/>
         <v>4.6631578947368419</v>
       </c>
     </row>
     <row r="46" ht="14.25">
-      <c r="A46" s="5">
+      <c r="A46" s="1">
         <v>44</v>
       </c>
       <c r="B46">
@@ -1885,20 +1896,20 @@
       <c r="C46">
         <v>89.700000000000003</v>
       </c>
-      <c r="D46">
-        <f>MAX(0,ROUND(B46/$H$2*224,1)-1)</f>
-        <v>223</v>
-      </c>
-      <c r="E46" s="2">
-        <f>MAX(0,ROUND(C46/$I$2*64,1)-1)</f>
+      <c r="D46" s="2">
+        <f>MAX(0,ROUND(B46/$K$2*224,1)-1)</f>
+        <v>81.400000000000006</v>
+      </c>
+      <c r="E46" s="3">
+        <f t="shared" si="3"/>
         <v>59.900000000000006</v>
       </c>
-      <c r="F46" s="3">
-        <f>B46/19</f>
+      <c r="F46" s="4">
+        <f t="shared" si="4"/>
         <v>7.3263157894736839</v>
       </c>
-      <c r="G46" s="4">
-        <f>C46/19</f>
+      <c r="G46" s="5">
+        <f t="shared" si="5"/>
         <v>4.7210526315789476</v>
       </c>
     </row>
@@ -1913,20 +1924,20 @@
       <c r="C47" s="6">
         <v>89.700000000000003</v>
       </c>
-      <c r="D47">
-        <f>MAX(0,ROUND(B47/$H$2*224,1)-1)</f>
-        <v>383.90000000000003</v>
-      </c>
-      <c r="E47" s="2">
-        <f>MAX(0,ROUND(C47/$I$2*64,1)-1)</f>
+      <c r="D47" s="2">
+        <f>MAX(0,ROUND(B47/$K$2*224,1)-1)</f>
+        <v>140.59999999999999</v>
+      </c>
+      <c r="E47" s="3">
+        <f t="shared" si="3"/>
         <v>59.900000000000006</v>
       </c>
-      <c r="F47" s="3">
-        <f>B47/19</f>
+      <c r="F47" s="4">
+        <f t="shared" si="4"/>
         <v>12.589473684210526</v>
       </c>
-      <c r="G47" s="4">
-        <f>C47/19</f>
+      <c r="G47" s="5">
+        <f t="shared" si="5"/>
         <v>4.7210526315789476</v>
       </c>
     </row>
@@ -1941,20 +1952,20 @@
       <c r="C48" s="6">
         <v>88.599999999999994</v>
       </c>
-      <c r="D48">
-        <f>MAX(0,ROUND(B48/$H$2*224,1)-1)</f>
-        <v>419.5</v>
-      </c>
-      <c r="E48" s="2">
-        <f>MAX(0,ROUND(C48/$I$2*64,1)-1)</f>
+      <c r="D48" s="2">
+        <f>MAX(0,ROUND(B48/$K$2*224,1)-1)</f>
+        <v>153.70000000000002</v>
+      </c>
+      <c r="E48" s="3">
+        <f t="shared" si="3"/>
         <v>59.200000000000003</v>
       </c>
-      <c r="F48" s="3">
-        <f>B48/19</f>
+      <c r="F48" s="4">
+        <f t="shared" si="4"/>
         <v>13.752631578947366</v>
       </c>
-      <c r="G48" s="4">
-        <f>C48/19</f>
+      <c r="G48" s="5">
+        <f t="shared" si="5"/>
         <v>4.6631578947368419</v>
       </c>
     </row>
@@ -1969,20 +1980,20 @@
       <c r="C49" s="6">
         <v>86</v>
       </c>
-      <c r="D49">
-        <f>MAX(0,ROUND(B49/$H$2*224,1)-1)</f>
-        <v>452</v>
-      </c>
-      <c r="E49" s="2">
-        <f>MAX(0,ROUND(C49/$I$2*64,1)-1)</f>
+      <c r="D49" s="2">
+        <f>MAX(0,ROUND(B49/$K$2*224,1)-1)</f>
+        <v>165.60000000000002</v>
+      </c>
+      <c r="E49" s="3">
+        <f t="shared" si="3"/>
         <v>57.400000000000006</v>
       </c>
-      <c r="F49" s="3">
-        <f>B49/19</f>
+      <c r="F49" s="4">
+        <f t="shared" si="4"/>
         <v>14.815789473684211</v>
       </c>
-      <c r="G49" s="4">
-        <f>C49/19</f>
+      <c r="G49" s="5">
+        <f t="shared" si="5"/>
         <v>4.5263157894736841</v>
       </c>
     </row>
@@ -1997,20 +2008,20 @@
       <c r="C50" s="6">
         <v>94.200000000000003</v>
       </c>
-      <c r="D50">
-        <f>MAX(0,ROUND(B50/$H$2*224,1)-1)</f>
-        <v>483.5</v>
-      </c>
-      <c r="E50" s="2">
-        <f>MAX(0,ROUND(C50/$I$2*64,1)-1)</f>
+      <c r="D50" s="2">
+        <f>MAX(0,ROUND(B50/$K$2*224,1)-1)</f>
+        <v>177.20000000000002</v>
+      </c>
+      <c r="E50" s="3">
+        <f t="shared" si="3"/>
         <v>63</v>
       </c>
-      <c r="F50" s="3">
-        <f>B50/19</f>
+      <c r="F50" s="4">
+        <f t="shared" si="4"/>
         <v>15.84736842105263</v>
       </c>
-      <c r="G50" s="4">
-        <f>C50/19</f>
+      <c r="G50" s="5">
+        <f t="shared" si="5"/>
         <v>4.9578947368421051</v>
       </c>
     </row>
@@ -2025,20 +2036,20 @@
       <c r="C51" s="6">
         <v>92.900000000000006</v>
       </c>
-      <c r="D51">
-        <f>MAX(0,ROUND(B51/$H$2*224,1)-1)</f>
-        <v>514.10000000000002</v>
-      </c>
-      <c r="E51" s="2">
+      <c r="D51" s="2">
+        <f>MAX(0,ROUND(B51/$K$2*224,1)-1)</f>
+        <v>188.5</v>
+      </c>
+      <c r="E51" s="3">
         <f>ROUND(C51/$I$2*64,1)-1</f>
         <v>62.100000000000001</v>
       </c>
-      <c r="F51" s="3">
-        <f>B51/19</f>
+      <c r="F51" s="4">
+        <f t="shared" si="4"/>
         <v>16.847368421052629</v>
       </c>
-      <c r="G51" s="4">
-        <f>C51/19</f>
+      <c r="G51" s="5">
+        <f t="shared" si="5"/>
         <v>4.8894736842105262</v>
       </c>
     </row>

</xml_diff>